<commit_message>
Adjusted RB points logic
</commit_message>
<xml_diff>
--- a/Files/Progression Regression Logic.xlsx
+++ b/Files/Progression Regression Logic.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethpe\OneDrive\Documents\Git\madden22stats\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40f61192ff96ff75/Documents/Git/madden22stats/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4525A2FD-8FCF-4C1C-8965-B5B6FED6E457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{4525A2FD-8FCF-4C1C-8965-B5B6FED6E457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA23FD7F-714E-4505-9CD8-3C6654752D63}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{54C2E4B7-FBFF-4F69-A3A4-847FA497B9AB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{54C2E4B7-FBFF-4F69-A3A4-847FA497B9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="ProReg" sheetId="2" r:id="rId1"/>
@@ -798,19 +798,19 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1131,56 +1131,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39242688-C415-4EFE-B0A8-90C7EAED6EC3}">
   <dimension ref="A1:AN119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I121" sqref="I121"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.54296875" customWidth="1"/>
-    <col min="4" max="4" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="26" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="9"/>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="9"/>
-      <c r="AF1" s="9"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
@@ -1191,7 +1189,7 @@
       <c r="AN1" s="1"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1202,47 +1200,47 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="7" t="s">
+      <c r="V2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
       <c r="Y2" s="2"/>
-      <c r="Z2" s="7" t="s">
+      <c r="Z2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
       <c r="AC2" s="2"/>
-      <c r="AD2" s="7" t="s">
+      <c r="AD2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
@@ -1253,7 +1251,7 @@
       <c r="AN2" s="2"/>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>65</v>
       </c>
@@ -1343,7 +1341,7 @@
       <c r="AN3" s="1"/>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A4" s="10"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>60</v>
       </c>
@@ -1433,7 +1431,7 @@
       <c r="AN4" s="1"/>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A5" s="10"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>61</v>
       </c>
@@ -1523,7 +1521,7 @@
       <c r="AN5" s="1"/>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="1" t="s">
         <v>62</v>
       </c>
@@ -1613,7 +1611,7 @@
       <c r="AN6" s="1"/>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A7" s="10"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1" t="s">
         <v>63</v>
       </c>
@@ -1703,7 +1701,7 @@
       <c r="AN7" s="1"/>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A8" s="10"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>64</v>
       </c>
@@ -1793,7 +1791,7 @@
       <c r="AN8" s="1"/>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="1" t="s">
         <v>54</v>
       </c>
@@ -1805,7 +1803,7 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>26</v>
@@ -1934,47 +1932,47 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="7" t="s">
+      <c r="N11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
       <c r="Q11" s="2"/>
-      <c r="R11" s="7" t="s">
+      <c r="R11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
       <c r="U11" s="2"/>
-      <c r="V11" s="7" t="s">
+      <c r="V11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
       <c r="Y11" s="2"/>
-      <c r="Z11" s="7" t="s">
+      <c r="Z11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="7"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="10"/>
       <c r="AC11" s="2"/>
-      <c r="AD11" s="7" t="s">
+      <c r="AD11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE11" s="7"/>
-      <c r="AF11" s="7"/>
+      <c r="AE11" s="10"/>
+      <c r="AF11" s="10"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
@@ -1985,7 +1983,7 @@
       <c r="AN11" s="2"/>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2061,7 +2059,7 @@
       <c r="AN12" s="1"/>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A13" s="10"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
         <v>82</v>
       </c>
@@ -2135,7 +2133,7 @@
       <c r="AN13" s="1"/>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="1" t="s">
         <v>83</v>
       </c>
@@ -2209,7 +2207,7 @@
       <c r="AN14" s="1"/>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="1" t="s">
         <v>84</v>
       </c>
@@ -2283,7 +2281,7 @@
       <c r="AN15" s="1"/>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="1" t="s">
         <v>85</v>
       </c>
@@ -2357,7 +2355,7 @@
       <c r="AN16" s="1"/>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="1" t="s">
         <v>92</v>
       </c>
@@ -2431,7 +2429,7 @@
       <c r="AN17" s="1"/>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A18" s="10"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="1" t="s">
         <v>93</v>
       </c>
@@ -2510,47 +2508,47 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="7" t="s">
+      <c r="J19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="7" t="s">
+      <c r="N19" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
       <c r="Q19" s="2"/>
-      <c r="R19" s="7" t="s">
+      <c r="R19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
       <c r="U19" s="2"/>
-      <c r="V19" s="7" t="s">
+      <c r="V19" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
       <c r="Y19" s="2"/>
-      <c r="Z19" s="7" t="s">
+      <c r="Z19" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA19" s="7"/>
-      <c r="AB19" s="7"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="10"/>
       <c r="AC19" s="2"/>
-      <c r="AD19" s="7" t="s">
+      <c r="AD19" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE19" s="7"/>
-      <c r="AF19" s="7"/>
+      <c r="AE19" s="10"/>
+      <c r="AF19" s="10"/>
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
@@ -2561,7 +2559,7 @@
       <c r="AN19" s="1"/>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2637,7 +2635,7 @@
       <c r="AN20" s="1"/>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A21" s="10"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="1" t="s">
         <v>94</v>
       </c>
@@ -2711,7 +2709,7 @@
       <c r="AN21" s="1"/>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A22" s="10"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="1" t="s">
         <v>95</v>
       </c>
@@ -2721,7 +2719,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>12</v>
@@ -2729,7 +2727,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>11</v>
@@ -2785,7 +2783,7 @@
       <c r="AN22" s="1"/>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A23" s="10"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="1" t="s">
         <v>99</v>
       </c>
@@ -2795,7 +2793,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>22</v>
@@ -2859,7 +2857,7 @@
       <c r="AN23" s="1"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A24" s="10"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="1" t="s">
         <v>98</v>
       </c>
@@ -2933,7 +2931,7 @@
       <c r="AN24" s="1"/>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A25" s="10"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="1" t="s">
         <v>97</v>
       </c>
@@ -3007,7 +3005,7 @@
       <c r="AN25" s="1"/>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A26" s="10"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="1" t="s">
         <v>96</v>
       </c>
@@ -3124,11 +3122,11 @@
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -3178,47 +3176,47 @@
         <v>57</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="7" t="s">
+      <c r="J29" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="7" t="s">
+      <c r="N29" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
       <c r="Q29" s="2"/>
-      <c r="R29" s="7" t="s">
+      <c r="R29" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
       <c r="U29" s="2"/>
-      <c r="V29" s="7" t="s">
+      <c r="V29" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W29" s="7"/>
-      <c r="X29" s="7"/>
+      <c r="W29" s="10"/>
+      <c r="X29" s="10"/>
       <c r="Y29" s="2"/>
-      <c r="Z29" s="7" t="s">
+      <c r="Z29" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA29" s="7"/>
-      <c r="AB29" s="7"/>
+      <c r="AA29" s="10"/>
+      <c r="AB29" s="10"/>
       <c r="AC29" s="2"/>
-      <c r="AD29" s="7" t="s">
+      <c r="AD29" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE29" s="7"/>
-      <c r="AF29" s="7"/>
+      <c r="AE29" s="10"/>
+      <c r="AF29" s="10"/>
       <c r="AG29" s="1"/>
       <c r="AH29" s="1"/>
       <c r="AI29" s="1"/>
@@ -3229,7 +3227,7 @@
       <c r="AN29" s="1"/>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -3321,7 +3319,7 @@
       <c r="AN30" s="1"/>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A31" s="10"/>
+      <c r="A31" s="8"/>
       <c r="B31" s="1" t="s">
         <v>183</v>
       </c>
@@ -3411,7 +3409,7 @@
       <c r="AN31" s="1"/>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A32" s="10"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="1" t="s">
         <v>184</v>
       </c>
@@ -3501,7 +3499,7 @@
       <c r="AN32" s="1"/>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A33" s="10"/>
+      <c r="A33" s="8"/>
       <c r="B33" s="1" t="s">
         <v>185</v>
       </c>
@@ -3591,7 +3589,7 @@
       <c r="AN33" s="1"/>
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A34" s="10"/>
+      <c r="A34" s="8"/>
       <c r="B34" s="1" t="s">
         <v>182</v>
       </c>
@@ -3681,7 +3679,7 @@
       <c r="AN34" s="1"/>
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A35" s="10"/>
+      <c r="A35" s="8"/>
       <c r="B35" s="1" t="s">
         <v>186</v>
       </c>
@@ -3771,7 +3769,7 @@
       <c r="AN35" s="1"/>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A36" s="10"/>
+      <c r="A36" s="8"/>
       <c r="B36" s="1" t="s">
         <v>181</v>
       </c>
@@ -3914,58 +3912,58 @@
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
       <c r="I38" s="2"/>
-      <c r="J38" s="7" t="s">
+      <c r="J38" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
       <c r="M38" s="2"/>
-      <c r="N38" s="7" t="s">
+      <c r="N38" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O38" s="7"/>
-      <c r="P38" s="7"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
       <c r="Q38" s="2"/>
-      <c r="R38" s="7" t="s">
+      <c r="R38" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S38" s="7"/>
-      <c r="T38" s="7"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
       <c r="U38" s="2"/>
-      <c r="V38" s="7" t="s">
+      <c r="V38" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W38" s="7"/>
-      <c r="X38" s="7"/>
+      <c r="W38" s="10"/>
+      <c r="X38" s="10"/>
       <c r="Y38" s="2"/>
-      <c r="Z38" s="7" t="s">
+      <c r="Z38" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA38" s="7"/>
-      <c r="AB38" s="7"/>
+      <c r="AA38" s="10"/>
+      <c r="AB38" s="10"/>
       <c r="AC38" s="2"/>
-      <c r="AD38" s="7" t="s">
+      <c r="AD38" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE38" s="7"/>
-      <c r="AF38" s="7"/>
+      <c r="AE38" s="10"/>
+      <c r="AF38" s="10"/>
       <c r="AG38" s="2"/>
       <c r="AH38" s="1"/>
       <c r="AI38" s="1"/>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
-      <c r="AL38" s="7"/>
-      <c r="AM38" s="7"/>
-      <c r="AN38" s="7"/>
+      <c r="AL38" s="10"/>
+      <c r="AM38" s="10"/>
+      <c r="AN38" s="10"/>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -4031,7 +4029,7 @@
         <v>48</v>
       </c>
       <c r="AF39" s="1"/>
-      <c r="AG39" s="10"/>
+      <c r="AG39" s="8"/>
       <c r="AH39" s="1"/>
       <c r="AI39" s="1"/>
       <c r="AJ39" s="1"/>
@@ -4041,7 +4039,7 @@
       <c r="AN39" s="1"/>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A40" s="10"/>
+      <c r="A40" s="8"/>
       <c r="B40" s="1" t="s">
         <v>111</v>
       </c>
@@ -4105,7 +4103,7 @@
         <v>31</v>
       </c>
       <c r="AF40" s="1"/>
-      <c r="AG40" s="10"/>
+      <c r="AG40" s="8"/>
       <c r="AH40" s="1"/>
       <c r="AI40" s="1"/>
       <c r="AJ40" s="1"/>
@@ -4115,7 +4113,7 @@
       <c r="AN40" s="1"/>
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A41" s="10"/>
+      <c r="A41" s="8"/>
       <c r="B41" s="1" t="s">
         <v>198</v>
       </c>
@@ -4179,7 +4177,7 @@
         <v>20</v>
       </c>
       <c r="AF41" s="1"/>
-      <c r="AG41" s="10"/>
+      <c r="AG41" s="8"/>
       <c r="AH41" s="1"/>
       <c r="AI41" s="1"/>
       <c r="AJ41" s="1"/>
@@ -4189,7 +4187,7 @@
       <c r="AN41" s="1"/>
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A42" s="10"/>
+      <c r="A42" s="8"/>
       <c r="B42" s="1" t="s">
         <v>199</v>
       </c>
@@ -4253,7 +4251,7 @@
         <v>28</v>
       </c>
       <c r="AF42" s="1"/>
-      <c r="AG42" s="10"/>
+      <c r="AG42" s="8"/>
       <c r="AH42" s="1"/>
       <c r="AI42" s="1"/>
       <c r="AJ42" s="1"/>
@@ -4263,7 +4261,7 @@
       <c r="AN42" s="1"/>
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A43" s="10"/>
+      <c r="A43" s="8"/>
       <c r="B43" s="1" t="s">
         <v>196</v>
       </c>
@@ -4327,7 +4325,7 @@
         <v>9</v>
       </c>
       <c r="AF43" s="1"/>
-      <c r="AG43" s="10"/>
+      <c r="AG43" s="8"/>
       <c r="AH43" s="1"/>
       <c r="AI43" s="1"/>
       <c r="AJ43" s="1"/>
@@ -4337,7 +4335,7 @@
       <c r="AN43" s="1"/>
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A44" s="10"/>
+      <c r="A44" s="8"/>
       <c r="B44" s="1" t="s">
         <v>197</v>
       </c>
@@ -4401,7 +4399,7 @@
         <v>10</v>
       </c>
       <c r="AF44" s="1"/>
-      <c r="AG44" s="10"/>
+      <c r="AG44" s="8"/>
       <c r="AH44" s="1"/>
       <c r="AI44" s="1"/>
       <c r="AJ44" s="1"/>
@@ -4411,7 +4409,7 @@
       <c r="AN44" s="1"/>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A45" s="10"/>
+      <c r="A45" s="8"/>
       <c r="B45" s="1" t="s">
         <v>72</v>
       </c>
@@ -4475,7 +4473,7 @@
         <v>12</v>
       </c>
       <c r="AF45" s="1"/>
-      <c r="AG45" s="10"/>
+      <c r="AG45" s="8"/>
       <c r="AH45" s="1"/>
       <c r="AI45" s="1"/>
       <c r="AJ45" s="1"/>
@@ -4536,47 +4534,47 @@
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="7" t="s">
+      <c r="F47" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
       <c r="I47" s="2"/>
-      <c r="J47" s="7" t="s">
+      <c r="J47" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="10"/>
       <c r="M47" s="2"/>
-      <c r="N47" s="7" t="s">
+      <c r="N47" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O47" s="7"/>
-      <c r="P47" s="7"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
       <c r="Q47" s="2"/>
-      <c r="R47" s="7" t="s">
+      <c r="R47" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S47" s="7"/>
-      <c r="T47" s="7"/>
+      <c r="S47" s="10"/>
+      <c r="T47" s="10"/>
       <c r="U47" s="2"/>
-      <c r="V47" s="7" t="s">
+      <c r="V47" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W47" s="7"/>
-      <c r="X47" s="7"/>
+      <c r="W47" s="10"/>
+      <c r="X47" s="10"/>
       <c r="Y47" s="2"/>
-      <c r="Z47" s="7" t="s">
+      <c r="Z47" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA47" s="7"/>
-      <c r="AB47" s="7"/>
+      <c r="AA47" s="10"/>
+      <c r="AB47" s="10"/>
       <c r="AC47" s="2"/>
-      <c r="AD47" s="7" t="s">
+      <c r="AD47" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE47" s="7"/>
-      <c r="AF47" s="7"/>
+      <c r="AE47" s="10"/>
+      <c r="AF47" s="10"/>
       <c r="AG47" s="1"/>
       <c r="AH47" s="1"/>
       <c r="AI47" s="1"/>
@@ -4587,7 +4585,7 @@
       <c r="AN47" s="1"/>
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -4663,7 +4661,7 @@
       <c r="AN48" s="1"/>
     </row>
     <row r="49" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A49" s="10"/>
+      <c r="A49" s="8"/>
       <c r="B49" s="1" t="s">
         <v>200</v>
       </c>
@@ -4737,7 +4735,7 @@
       <c r="AN49" s="1"/>
     </row>
     <row r="50" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A50" s="10"/>
+      <c r="A50" s="8"/>
       <c r="B50" s="1" t="s">
         <v>112</v>
       </c>
@@ -4811,7 +4809,7 @@
       <c r="AN50" s="1"/>
     </row>
     <row r="51" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A51" s="10"/>
+      <c r="A51" s="8"/>
       <c r="B51" s="1" t="s">
         <v>117</v>
       </c>
@@ -4885,7 +4883,7 @@
       <c r="AN51" s="1"/>
     </row>
     <row r="52" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A52" s="10"/>
+      <c r="A52" s="8"/>
       <c r="B52" s="1" t="s">
         <v>118</v>
       </c>
@@ -4959,7 +4957,7 @@
       <c r="AN52" s="1"/>
     </row>
     <row r="53" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A53" s="10"/>
+      <c r="A53" s="8"/>
       <c r="B53" s="1" t="s">
         <v>197</v>
       </c>
@@ -5033,7 +5031,7 @@
       <c r="AN53" s="1"/>
     </row>
     <row r="54" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A54" s="10"/>
+      <c r="A54" s="8"/>
       <c r="B54" s="1" t="s">
         <v>72</v>
       </c>
@@ -5162,47 +5160,47 @@
         <v>110</v>
       </c>
       <c r="E56" s="1"/>
-      <c r="F56" s="7" t="s">
+      <c r="F56" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
       <c r="I56" s="2"/>
-      <c r="J56" s="7" t="s">
+      <c r="J56" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K56" s="7"/>
-      <c r="L56" s="7"/>
+      <c r="K56" s="10"/>
+      <c r="L56" s="10"/>
       <c r="M56" s="2"/>
-      <c r="N56" s="7" t="s">
+      <c r="N56" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O56" s="7"/>
-      <c r="P56" s="7"/>
+      <c r="O56" s="10"/>
+      <c r="P56" s="10"/>
       <c r="Q56" s="2"/>
-      <c r="R56" s="7" t="s">
+      <c r="R56" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S56" s="7"/>
-      <c r="T56" s="7"/>
+      <c r="S56" s="10"/>
+      <c r="T56" s="10"/>
       <c r="U56" s="2"/>
-      <c r="V56" s="7" t="s">
+      <c r="V56" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W56" s="7"/>
-      <c r="X56" s="7"/>
+      <c r="W56" s="10"/>
+      <c r="X56" s="10"/>
       <c r="Y56" s="2"/>
-      <c r="Z56" s="7" t="s">
+      <c r="Z56" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA56" s="7"/>
-      <c r="AB56" s="7"/>
+      <c r="AA56" s="10"/>
+      <c r="AB56" s="10"/>
       <c r="AC56" s="2"/>
-      <c r="AD56" s="7" t="s">
+      <c r="AD56" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE56" s="7"/>
-      <c r="AF56" s="7"/>
+      <c r="AE56" s="10"/>
+      <c r="AF56" s="10"/>
       <c r="AG56" s="1"/>
       <c r="AH56" s="1"/>
       <c r="AI56" s="1"/>
@@ -5213,7 +5211,7 @@
       <c r="AN56" s="1"/>
     </row>
     <row r="57" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A57" s="10" t="s">
+      <c r="A57" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -5305,7 +5303,7 @@
       <c r="AN57" s="1"/>
     </row>
     <row r="58" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A58" s="10"/>
+      <c r="A58" s="8"/>
       <c r="B58" s="1" t="s">
         <v>115</v>
       </c>
@@ -5395,7 +5393,7 @@
       <c r="AN58" s="1"/>
     </row>
     <row r="59" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A59" s="10"/>
+      <c r="A59" s="8"/>
       <c r="B59" s="1" t="s">
         <v>116</v>
       </c>
@@ -5485,7 +5483,7 @@
       <c r="AN59" s="1"/>
     </row>
     <row r="60" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A60" s="10"/>
+      <c r="A60" s="8"/>
       <c r="B60" s="1" t="s">
         <v>113</v>
       </c>
@@ -5575,7 +5573,7 @@
       <c r="AN60" s="1"/>
     </row>
     <row r="61" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A61" s="10"/>
+      <c r="A61" s="8"/>
       <c r="B61" s="1" t="s">
         <v>114</v>
       </c>
@@ -5665,7 +5663,7 @@
       <c r="AN61" s="1"/>
     </row>
     <row r="62" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A62" s="10"/>
+      <c r="A62" s="8"/>
       <c r="B62" s="1" t="s">
         <v>203</v>
       </c>
@@ -5755,7 +5753,7 @@
       <c r="AN62" s="1"/>
     </row>
     <row r="63" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A63" s="10"/>
+      <c r="A63" s="8"/>
       <c r="B63" s="1" t="s">
         <v>102</v>
       </c>
@@ -5898,47 +5896,47 @@
         <v>201</v>
       </c>
       <c r="E65" s="1"/>
-      <c r="F65" s="7" t="s">
+      <c r="F65" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G65" s="7"/>
-      <c r="H65" s="7"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
       <c r="I65" s="2"/>
-      <c r="J65" s="7" t="s">
+      <c r="J65" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K65" s="7"/>
-      <c r="L65" s="7"/>
+      <c r="K65" s="10"/>
+      <c r="L65" s="10"/>
       <c r="M65" s="2"/>
-      <c r="N65" s="7" t="s">
+      <c r="N65" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O65" s="7"/>
-      <c r="P65" s="7"/>
+      <c r="O65" s="10"/>
+      <c r="P65" s="10"/>
       <c r="Q65" s="2"/>
-      <c r="R65" s="7" t="s">
+      <c r="R65" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S65" s="7"/>
-      <c r="T65" s="7"/>
+      <c r="S65" s="10"/>
+      <c r="T65" s="10"/>
       <c r="U65" s="2"/>
-      <c r="V65" s="7" t="s">
+      <c r="V65" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W65" s="7"/>
-      <c r="X65" s="7"/>
+      <c r="W65" s="10"/>
+      <c r="X65" s="10"/>
       <c r="Y65" s="2"/>
-      <c r="Z65" s="7" t="s">
+      <c r="Z65" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA65" s="7"/>
-      <c r="AB65" s="7"/>
+      <c r="AA65" s="10"/>
+      <c r="AB65" s="10"/>
       <c r="AC65" s="2"/>
-      <c r="AD65" s="7" t="s">
+      <c r="AD65" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE65" s="7"/>
-      <c r="AF65" s="7"/>
+      <c r="AE65" s="10"/>
+      <c r="AF65" s="10"/>
       <c r="AG65" s="1"/>
       <c r="AH65" s="1"/>
       <c r="AI65" s="1"/>
@@ -5949,7 +5947,7 @@
       <c r="AN65" s="1"/>
     </row>
     <row r="66" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -6041,7 +6039,7 @@
       <c r="AN66" s="1"/>
     </row>
     <row r="67" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A67" s="10"/>
+      <c r="A67" s="8"/>
       <c r="B67" s="1" t="s">
         <v>126</v>
       </c>
@@ -6131,7 +6129,7 @@
       <c r="AN67" s="1"/>
     </row>
     <row r="68" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A68" s="10"/>
+      <c r="A68" s="8"/>
       <c r="B68" s="1" t="s">
         <v>206</v>
       </c>
@@ -6221,7 +6219,7 @@
       <c r="AN68" s="1"/>
     </row>
     <row r="69" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A69" s="10"/>
+      <c r="A69" s="8"/>
       <c r="B69" s="1" t="s">
         <v>204</v>
       </c>
@@ -6311,7 +6309,7 @@
       <c r="AN69" s="1"/>
     </row>
     <row r="70" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A70" s="10"/>
+      <c r="A70" s="8"/>
       <c r="B70" s="1" t="s">
         <v>123</v>
       </c>
@@ -6401,7 +6399,7 @@
       <c r="AN70" s="1"/>
     </row>
     <row r="71" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A71" s="10"/>
+      <c r="A71" s="8"/>
       <c r="B71" s="1" t="s">
         <v>124</v>
       </c>
@@ -6491,7 +6489,7 @@
       <c r="AN71" s="1"/>
     </row>
     <row r="72" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A72" s="10"/>
+      <c r="A72" s="8"/>
       <c r="B72" s="1" t="s">
         <v>125</v>
       </c>
@@ -6624,9 +6622,9 @@
     </row>
     <row r="74" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -6672,47 +6670,47 @@
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="7" t="s">
+      <c r="F75" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G75" s="7"/>
-      <c r="H75" s="7"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
       <c r="I75" s="2"/>
-      <c r="J75" s="7" t="s">
+      <c r="J75" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K75" s="7"/>
-      <c r="L75" s="7"/>
+      <c r="K75" s="10"/>
+      <c r="L75" s="10"/>
       <c r="M75" s="2"/>
-      <c r="N75" s="7" t="s">
+      <c r="N75" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O75" s="7"/>
-      <c r="P75" s="7"/>
+      <c r="O75" s="10"/>
+      <c r="P75" s="10"/>
       <c r="Q75" s="2"/>
-      <c r="R75" s="7" t="s">
+      <c r="R75" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S75" s="7"/>
-      <c r="T75" s="7"/>
+      <c r="S75" s="10"/>
+      <c r="T75" s="10"/>
       <c r="U75" s="2"/>
-      <c r="V75" s="7" t="s">
+      <c r="V75" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W75" s="7"/>
-      <c r="X75" s="7"/>
+      <c r="W75" s="10"/>
+      <c r="X75" s="10"/>
       <c r="Y75" s="2"/>
-      <c r="Z75" s="7" t="s">
+      <c r="Z75" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA75" s="7"/>
-      <c r="AB75" s="7"/>
+      <c r="AA75" s="10"/>
+      <c r="AB75" s="10"/>
       <c r="AC75" s="2"/>
-      <c r="AD75" s="7" t="s">
+      <c r="AD75" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE75" s="7"/>
-      <c r="AF75" s="7"/>
+      <c r="AE75" s="10"/>
+      <c r="AF75" s="10"/>
       <c r="AG75" s="1"/>
       <c r="AH75" s="1"/>
       <c r="AI75" s="1"/>
@@ -6723,7 +6721,7 @@
       <c r="AN75" s="1"/>
     </row>
     <row r="76" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="8" t="s">
         <v>50</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -6815,7 +6813,7 @@
       <c r="AN76" s="1"/>
     </row>
     <row r="77" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A77" s="10"/>
+      <c r="A77" s="8"/>
       <c r="B77" s="1" t="s">
         <v>53</v>
       </c>
@@ -6905,7 +6903,7 @@
       <c r="AN77" s="1"/>
     </row>
     <row r="78" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A78" s="10"/>
+      <c r="A78" s="8"/>
       <c r="B78" s="1" t="s">
         <v>40</v>
       </c>
@@ -6995,7 +6993,7 @@
       <c r="AN78" s="1"/>
     </row>
     <row r="79" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A79" s="10"/>
+      <c r="A79" s="8"/>
       <c r="B79" s="1" t="s">
         <v>34</v>
       </c>
@@ -7085,7 +7083,7 @@
       <c r="AN79" s="1"/>
     </row>
     <row r="80" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A80" s="10"/>
+      <c r="A80" s="8"/>
       <c r="B80" s="1" t="s">
         <v>35</v>
       </c>
@@ -7175,7 +7173,7 @@
       <c r="AN80" s="1"/>
     </row>
     <row r="81" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A81" s="10"/>
+      <c r="A81" s="8"/>
       <c r="B81" s="1" t="s">
         <v>11</v>
       </c>
@@ -7187,13 +7185,13 @@
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="I81" s="1"/>
       <c r="J81" s="1" t="s">
@@ -7265,7 +7263,7 @@
       <c r="AN81" s="1"/>
     </row>
     <row r="82" spans="1:40" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="10"/>
+      <c r="A82" s="8"/>
       <c r="B82" s="1" t="s">
         <v>12</v>
       </c>
@@ -7398,9 +7396,9 @@
     </row>
     <row r="84" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
-      <c r="B84" s="11"/>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
@@ -7448,47 +7446,47 @@
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
-      <c r="F85" s="7" t="s">
+      <c r="F85" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G85" s="7"/>
-      <c r="H85" s="7"/>
+      <c r="G85" s="10"/>
+      <c r="H85" s="10"/>
       <c r="I85" s="2"/>
-      <c r="J85" s="7" t="s">
+      <c r="J85" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K85" s="7"/>
-      <c r="L85" s="7"/>
+      <c r="K85" s="10"/>
+      <c r="L85" s="10"/>
       <c r="M85" s="2"/>
-      <c r="N85" s="7" t="s">
+      <c r="N85" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O85" s="7"/>
-      <c r="P85" s="7"/>
+      <c r="O85" s="10"/>
+      <c r="P85" s="10"/>
       <c r="Q85" s="2"/>
-      <c r="R85" s="7" t="s">
+      <c r="R85" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S85" s="7"/>
-      <c r="T85" s="7"/>
+      <c r="S85" s="10"/>
+      <c r="T85" s="10"/>
       <c r="U85" s="2"/>
-      <c r="V85" s="7" t="s">
+      <c r="V85" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W85" s="7"/>
-      <c r="X85" s="7"/>
+      <c r="W85" s="10"/>
+      <c r="X85" s="10"/>
       <c r="Y85" s="2"/>
-      <c r="Z85" s="7" t="s">
+      <c r="Z85" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA85" s="7"/>
-      <c r="AB85" s="7"/>
+      <c r="AA85" s="10"/>
+      <c r="AB85" s="10"/>
       <c r="AC85" s="2"/>
-      <c r="AD85" s="7" t="s">
+      <c r="AD85" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE85" s="7"/>
-      <c r="AF85" s="7"/>
+      <c r="AE85" s="10"/>
+      <c r="AF85" s="10"/>
       <c r="AG85" s="1"/>
       <c r="AH85" s="1"/>
       <c r="AI85" s="1"/>
@@ -7499,7 +7497,7 @@
       <c r="AN85" s="1"/>
     </row>
     <row r="86" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A86" s="10" t="s">
+      <c r="A86" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -7591,7 +7589,7 @@
       <c r="AN86" s="1"/>
     </row>
     <row r="87" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A87" s="10"/>
+      <c r="A87" s="8"/>
       <c r="B87" s="1" t="s">
         <v>218</v>
       </c>
@@ -7681,7 +7679,7 @@
       <c r="AN87" s="1"/>
     </row>
     <row r="88" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A88" s="10"/>
+      <c r="A88" s="8"/>
       <c r="B88" s="1" t="s">
         <v>34</v>
       </c>
@@ -7771,7 +7769,7 @@
       <c r="AN88" s="1"/>
     </row>
     <row r="89" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A89" s="10"/>
+      <c r="A89" s="8"/>
       <c r="B89" s="1" t="s">
         <v>9</v>
       </c>
@@ -7861,7 +7859,7 @@
       <c r="AN89" s="1"/>
     </row>
     <row r="90" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A90" s="10"/>
+      <c r="A90" s="8"/>
       <c r="B90" s="1" t="s">
         <v>10</v>
       </c>
@@ -7951,7 +7949,7 @@
       <c r="AN90" s="1"/>
     </row>
     <row r="91" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A91" s="10"/>
+      <c r="A91" s="8"/>
       <c r="B91" s="1" t="s">
         <v>11</v>
       </c>
@@ -8041,7 +8039,7 @@
       <c r="AN91" s="1"/>
     </row>
     <row r="92" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A92" s="10"/>
+      <c r="A92" s="8"/>
       <c r="B92" s="1" t="s">
         <v>12</v>
       </c>
@@ -8180,29 +8178,29 @@
         <v>222</v>
       </c>
       <c r="E94" s="1"/>
-      <c r="F94" s="7" t="s">
+      <c r="F94" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
+      <c r="G94" s="10"/>
+      <c r="H94" s="10"/>
       <c r="I94" s="2"/>
-      <c r="J94" s="7" t="s">
+      <c r="J94" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K94" s="7"/>
-      <c r="L94" s="7"/>
+      <c r="K94" s="10"/>
+      <c r="L94" s="10"/>
       <c r="M94" s="2"/>
-      <c r="N94" s="7" t="s">
+      <c r="N94" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="O94" s="7"/>
-      <c r="P94" s="7"/>
+      <c r="O94" s="10"/>
+      <c r="P94" s="10"/>
       <c r="Q94" s="2"/>
-      <c r="R94" s="7" t="s">
+      <c r="R94" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="S94" s="7"/>
-      <c r="T94" s="7"/>
+      <c r="S94" s="10"/>
+      <c r="T94" s="10"/>
       <c r="U94" s="1"/>
       <c r="V94" s="1"/>
       <c r="W94" s="1"/>
@@ -8225,7 +8223,7 @@
       <c r="AN94" s="1"/>
     </row>
     <row r="95" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="8" t="s">
+      <c r="A95" s="9" t="s">
         <v>138</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -8299,7 +8297,7 @@
       <c r="AN95" s="1"/>
     </row>
     <row r="96" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="8"/>
+      <c r="A96" s="9"/>
       <c r="B96" s="1" t="s">
         <v>145</v>
       </c>
@@ -8371,7 +8369,7 @@
       <c r="AN96" s="1"/>
     </row>
     <row r="97" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="8"/>
+      <c r="A97" s="9"/>
       <c r="B97" s="1" t="s">
         <v>146</v>
       </c>
@@ -8443,7 +8441,7 @@
       <c r="AN97" s="1"/>
     </row>
     <row r="98" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="8"/>
+      <c r="A98" s="9"/>
       <c r="B98" s="1" t="s">
         <v>147</v>
       </c>
@@ -8515,7 +8513,7 @@
       <c r="AN98" s="1"/>
     </row>
     <row r="99" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="8"/>
+      <c r="A99" s="9"/>
       <c r="B99" s="1" t="s">
         <v>148</v>
       </c>
@@ -8587,7 +8585,7 @@
       <c r="AN99" s="1"/>
     </row>
     <row r="100" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="8"/>
+      <c r="A100" s="9"/>
       <c r="B100" s="1" t="s">
         <v>149</v>
       </c>
@@ -8659,7 +8657,7 @@
       <c r="AN100" s="1"/>
     </row>
     <row r="101" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="8"/>
+      <c r="A101" s="9"/>
       <c r="B101" s="1" t="s">
         <v>150</v>
       </c>
@@ -8778,29 +8776,29 @@
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
-      <c r="F103" s="7" t="s">
+      <c r="F103" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="G103" s="7"/>
-      <c r="H103" s="7"/>
+      <c r="G103" s="10"/>
+      <c r="H103" s="10"/>
       <c r="I103" s="2"/>
-      <c r="J103" s="7" t="s">
+      <c r="J103" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K103" s="7"/>
-      <c r="L103" s="7"/>
+      <c r="K103" s="10"/>
+      <c r="L103" s="10"/>
       <c r="M103" s="2"/>
-      <c r="N103" s="7" t="s">
+      <c r="N103" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="O103" s="7"/>
-      <c r="P103" s="7"/>
+      <c r="O103" s="10"/>
+      <c r="P103" s="10"/>
       <c r="Q103" s="2"/>
-      <c r="R103" s="7" t="s">
+      <c r="R103" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="S103" s="7"/>
-      <c r="T103" s="7"/>
+      <c r="S103" s="10"/>
+      <c r="T103" s="10"/>
       <c r="U103" s="1"/>
       <c r="V103" s="1"/>
       <c r="W103" s="1"/>
@@ -8823,7 +8821,7 @@
       <c r="AN103" s="1"/>
     </row>
     <row r="104" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="8" t="s">
+      <c r="A104" s="9" t="s">
         <v>162</v>
       </c>
       <c r="B104" s="1" t="s">
@@ -8889,7 +8887,7 @@
       <c r="AN104" s="1"/>
     </row>
     <row r="105" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="8"/>
+      <c r="A105" s="9"/>
       <c r="B105" s="1" t="s">
         <v>12</v>
       </c>
@@ -8961,7 +8959,7 @@
       <c r="AN105" s="1"/>
     </row>
     <row r="106" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="8"/>
+      <c r="A106" s="9"/>
       <c r="B106" s="1" t="s">
         <v>102</v>
       </c>
@@ -9033,7 +9031,7 @@
       <c r="AN106" s="1"/>
     </row>
     <row r="107" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="8"/>
+      <c r="A107" s="9"/>
       <c r="B107" s="1" t="s">
         <v>167</v>
       </c>
@@ -9105,7 +9103,7 @@
       <c r="AN107" s="1"/>
     </row>
     <row r="108" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="8"/>
+      <c r="A108" s="9"/>
       <c r="B108" s="1" t="s">
         <v>166</v>
       </c>
@@ -9177,7 +9175,7 @@
       <c r="AN108" s="1"/>
     </row>
     <row r="109" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="8"/>
+      <c r="A109" s="9"/>
       <c r="B109" s="1" t="s">
         <v>164</v>
       </c>
@@ -9249,7 +9247,7 @@
       <c r="AN109" s="1"/>
     </row>
     <row r="110" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="8"/>
+      <c r="A110" s="9"/>
       <c r="B110" s="1" t="s">
         <v>165</v>
       </c>
@@ -9321,7 +9319,7 @@
       <c r="AN110" s="1"/>
     </row>
     <row r="112" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A112" s="8" t="s">
+      <c r="A112" s="9" t="s">
         <v>74</v>
       </c>
       <c r="B112" s="1"/>
@@ -9346,7 +9344,7 @@
       <c r="I112" s="12"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A113" s="8"/>
+      <c r="A113" s="9"/>
       <c r="B113" s="1" t="s">
         <v>13</v>
       </c>
@@ -9369,7 +9367,7 @@
       <c r="I113" s="12"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A114" s="8"/>
+      <c r="A114" s="9"/>
       <c r="B114" s="1" t="s">
         <v>17</v>
       </c>
@@ -9392,7 +9390,7 @@
       <c r="I114" s="12"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A115" s="8"/>
+      <c r="A115" s="9"/>
       <c r="B115" s="1" t="s">
         <v>21</v>
       </c>
@@ -9415,7 +9413,7 @@
       <c r="I115" s="12"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A116" s="8"/>
+      <c r="A116" s="9"/>
       <c r="B116" s="1" t="s">
         <v>23</v>
       </c>
@@ -9438,7 +9436,7 @@
       <c r="I116" s="12"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A117" s="8"/>
+      <c r="A117" s="9"/>
       <c r="B117" s="1" t="s">
         <v>25</v>
       </c>
@@ -9461,7 +9459,7 @@
       <c r="I117" s="12"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A118" s="8"/>
+      <c r="A118" s="9"/>
       <c r="B118" s="1" t="s">
         <v>30</v>
       </c>
@@ -9484,7 +9482,7 @@
       <c r="I118" s="12"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A119" s="8"/>
+      <c r="A119" s="9"/>
       <c r="B119" s="1" t="s">
         <v>75</v>
       </c>
@@ -9508,14 +9506,82 @@
     </row>
   </sheetData>
   <mergeCells count="99">
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="A86:A92"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A66:A72"/>
-    <mergeCell ref="A57:A63"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="R94:T94"/>
+    <mergeCell ref="A95:A101"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="J103:L103"/>
+    <mergeCell ref="N103:P103"/>
+    <mergeCell ref="R103:T103"/>
+    <mergeCell ref="A112:A119"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="J94:L94"/>
+    <mergeCell ref="N94:P94"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="H112:I119"/>
+    <mergeCell ref="F1:AF1"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="AD11:AF11"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="V19:X19"/>
+    <mergeCell ref="Z19:AB19"/>
+    <mergeCell ref="AD19:AF19"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="V11:X11"/>
+    <mergeCell ref="Z11:AB11"/>
+    <mergeCell ref="Z29:AB29"/>
+    <mergeCell ref="AD29:AF29"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="N38:P38"/>
+    <mergeCell ref="R38:T38"/>
+    <mergeCell ref="V38:X38"/>
+    <mergeCell ref="Z38:AB38"/>
+    <mergeCell ref="AD38:AF38"/>
+    <mergeCell ref="V29:X29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="R29:T29"/>
+    <mergeCell ref="AL38:AN38"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="AG39:AG45"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="J47:L47"/>
+    <mergeCell ref="N47:P47"/>
+    <mergeCell ref="R47:T47"/>
+    <mergeCell ref="V47:X47"/>
+    <mergeCell ref="Z47:AB47"/>
+    <mergeCell ref="AD47:AF47"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="J65:L65"/>
+    <mergeCell ref="N65:P65"/>
+    <mergeCell ref="R65:T65"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="J56:L56"/>
+    <mergeCell ref="N56:P56"/>
+    <mergeCell ref="R56:T56"/>
+    <mergeCell ref="Z56:AB56"/>
+    <mergeCell ref="AD56:AF56"/>
+    <mergeCell ref="V65:X65"/>
+    <mergeCell ref="Z65:AB65"/>
+    <mergeCell ref="AD65:AF65"/>
+    <mergeCell ref="V56:X56"/>
     <mergeCell ref="Z75:AB75"/>
     <mergeCell ref="AD75:AF75"/>
     <mergeCell ref="A76:A82"/>
@@ -9531,82 +9597,14 @@
     <mergeCell ref="N75:P75"/>
     <mergeCell ref="R75:T75"/>
     <mergeCell ref="V75:X75"/>
-    <mergeCell ref="Z56:AB56"/>
-    <mergeCell ref="AD56:AF56"/>
-    <mergeCell ref="V65:X65"/>
-    <mergeCell ref="Z65:AB65"/>
-    <mergeCell ref="AD65:AF65"/>
-    <mergeCell ref="V56:X56"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="J65:L65"/>
-    <mergeCell ref="N65:P65"/>
-    <mergeCell ref="R65:T65"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="J56:L56"/>
-    <mergeCell ref="N56:P56"/>
-    <mergeCell ref="R56:T56"/>
-    <mergeCell ref="AL38:AN38"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="AG39:AG45"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="J47:L47"/>
-    <mergeCell ref="N47:P47"/>
-    <mergeCell ref="R47:T47"/>
-    <mergeCell ref="V47:X47"/>
-    <mergeCell ref="Z47:AB47"/>
-    <mergeCell ref="AD47:AF47"/>
-    <mergeCell ref="Z29:AB29"/>
-    <mergeCell ref="AD29:AF29"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="N38:P38"/>
-    <mergeCell ref="R38:T38"/>
-    <mergeCell ref="V38:X38"/>
-    <mergeCell ref="Z38:AB38"/>
-    <mergeCell ref="AD38:AF38"/>
-    <mergeCell ref="V29:X29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="AD11:AF11"/>
-    <mergeCell ref="A12:A18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="V19:X19"/>
-    <mergeCell ref="Z19:AB19"/>
-    <mergeCell ref="AD19:AF19"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="V11:X11"/>
-    <mergeCell ref="Z11:AB11"/>
-    <mergeCell ref="F1:AF1"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="AD2:AF2"/>
-    <mergeCell ref="A112:A119"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="J94:L94"/>
-    <mergeCell ref="N94:P94"/>
-    <mergeCell ref="A104:A110"/>
-    <mergeCell ref="H112:I119"/>
-    <mergeCell ref="R94:T94"/>
-    <mergeCell ref="A95:A101"/>
-    <mergeCell ref="F103:H103"/>
-    <mergeCell ref="J103:L103"/>
-    <mergeCell ref="N103:P103"/>
-    <mergeCell ref="R103:T103"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="A86:A92"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="A57:A63"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed prog & reg points
</commit_message>
<xml_diff>
--- a/Files/Progression Regression Logic.xlsx
+++ b/Files/Progression Regression Logic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40f61192ff96ff75/Documents/Git/madden22stats/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{4525A2FD-8FCF-4C1C-8965-B5B6FED6E457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA23FD7F-714E-4505-9CD8-3C6654752D63}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{4525A2FD-8FCF-4C1C-8965-B5B6FED6E457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12B6243F-1607-4AD2-A93C-631464DF2271}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{54C2E4B7-FBFF-4F69-A3A4-847FA497B9AB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{54C2E4B7-FBFF-4F69-A3A4-847FA497B9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="ProReg" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="226">
   <si>
     <t>Yards</t>
   </si>
@@ -706,6 +706,12 @@
   </si>
   <si>
     <t>Games Played</t>
+  </si>
+  <si>
+    <t>-15</t>
+  </si>
+  <si>
+    <t>-13</t>
   </si>
 </sst>
 </file>
@@ -798,22 +804,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1131,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39242688-C415-4EFE-B0A8-90C7EAED6EC3}">
   <dimension ref="A1:AN119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1143,42 +1149,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="26" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="11" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
@@ -1189,7 +1195,7 @@
       <c r="AN1" s="1"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1200,47 +1206,47 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="10" t="s">
+      <c r="R2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="10" t="s">
+      <c r="V2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
       <c r="Y2" s="2"/>
-      <c r="Z2" s="10" t="s">
+      <c r="Z2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
       <c r="AC2" s="2"/>
-      <c r="AD2" s="10" t="s">
+      <c r="AD2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
@@ -1251,7 +1257,7 @@
       <c r="AN2" s="2"/>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A3" s="8"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="1" t="s">
         <v>65</v>
       </c>
@@ -1341,7 +1347,7 @@
       <c r="AN3" s="1"/>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A4" s="8"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="1" t="s">
         <v>60</v>
       </c>
@@ -1431,7 +1437,7 @@
       <c r="AN4" s="1"/>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A5" s="8"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="1" t="s">
         <v>61</v>
       </c>
@@ -1443,7 +1449,7 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>12</v>
@@ -1521,7 +1527,7 @@
       <c r="AN5" s="1"/>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A6" s="8"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="1" t="s">
         <v>62</v>
       </c>
@@ -1533,7 +1539,7 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>16</v>
@@ -1611,7 +1617,7 @@
       <c r="AN6" s="1"/>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A7" s="8"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="1" t="s">
         <v>63</v>
       </c>
@@ -1623,7 +1629,7 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>7</v>
@@ -1701,7 +1707,7 @@
       <c r="AN7" s="1"/>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A8" s="8"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="1" t="s">
         <v>64</v>
       </c>
@@ -1713,7 +1719,7 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>18</v>
@@ -1723,7 +1729,7 @@
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>14</v>
@@ -1791,7 +1797,7 @@
       <c r="AN8" s="1"/>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A9" s="8"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="1" t="s">
         <v>54</v>
       </c>
@@ -1803,7 +1809,7 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>4</v>
+        <v>224</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>26</v>
@@ -1813,7 +1819,7 @@
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>6</v>
@@ -1932,47 +1938,47 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="10" t="s">
+      <c r="N11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
       <c r="Q11" s="2"/>
-      <c r="R11" s="10" t="s">
+      <c r="R11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
       <c r="U11" s="2"/>
-      <c r="V11" s="10" t="s">
+      <c r="V11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W11" s="10"/>
-      <c r="X11" s="10"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
       <c r="Y11" s="2"/>
-      <c r="Z11" s="10" t="s">
+      <c r="Z11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA11" s="10"/>
-      <c r="AB11" s="10"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
       <c r="AC11" s="2"/>
-      <c r="AD11" s="10" t="s">
+      <c r="AD11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE11" s="10"/>
-      <c r="AF11" s="10"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
@@ -1983,7 +1989,7 @@
       <c r="AN11" s="2"/>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2059,7 +2065,7 @@
       <c r="AN12" s="1"/>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A13" s="8"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="1" t="s">
         <v>82</v>
       </c>
@@ -2133,7 +2139,7 @@
       <c r="AN13" s="1"/>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A14" s="8"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="1" t="s">
         <v>83</v>
       </c>
@@ -2207,7 +2213,7 @@
       <c r="AN14" s="1"/>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A15" s="8"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="1" t="s">
         <v>84</v>
       </c>
@@ -2281,7 +2287,7 @@
       <c r="AN15" s="1"/>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A16" s="8"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="1" t="s">
         <v>85</v>
       </c>
@@ -2291,7 +2297,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>7</v>
@@ -2339,7 +2345,7 @@
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="AE16" s="1" t="s">
         <v>8</v>
@@ -2355,7 +2361,7 @@
       <c r="AN16" s="1"/>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="1" t="s">
         <v>92</v>
       </c>
@@ -2365,7 +2371,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>18</v>
@@ -2413,7 +2419,7 @@
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AE17" s="1" t="s">
         <v>10</v>
@@ -2429,7 +2435,7 @@
       <c r="AN17" s="1"/>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A18" s="8"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="1" t="s">
         <v>93</v>
       </c>
@@ -2439,7 +2445,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>4</v>
+        <v>224</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>26</v>
@@ -2487,7 +2493,7 @@
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
       <c r="AD18" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="AE18" s="1" t="s">
         <v>12</v>
@@ -2508,47 +2514,47 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="10" t="s">
+      <c r="N19" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
       <c r="Q19" s="2"/>
-      <c r="R19" s="10" t="s">
+      <c r="R19" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
       <c r="U19" s="2"/>
-      <c r="V19" s="10" t="s">
+      <c r="V19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W19" s="10"/>
-      <c r="X19" s="10"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
       <c r="Y19" s="2"/>
-      <c r="Z19" s="10" t="s">
+      <c r="Z19" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA19" s="10"/>
-      <c r="AB19" s="10"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7"/>
       <c r="AC19" s="2"/>
-      <c r="AD19" s="10" t="s">
+      <c r="AD19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE19" s="10"/>
-      <c r="AF19" s="10"/>
+      <c r="AE19" s="7"/>
+      <c r="AF19" s="7"/>
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
@@ -2559,7 +2565,7 @@
       <c r="AN19" s="1"/>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2635,7 +2641,7 @@
       <c r="AN20" s="1"/>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A21" s="8"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="1" t="s">
         <v>94</v>
       </c>
@@ -2709,7 +2715,7 @@
       <c r="AN21" s="1"/>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A22" s="8"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="1" t="s">
         <v>95</v>
       </c>
@@ -2783,7 +2789,7 @@
       <c r="AN22" s="1"/>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A23" s="8"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="1" t="s">
         <v>99</v>
       </c>
@@ -2857,7 +2863,7 @@
       <c r="AN23" s="1"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A24" s="8"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="1" t="s">
         <v>98</v>
       </c>
@@ -2915,7 +2921,7 @@
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
       <c r="AD24" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="AE24" s="1" t="s">
         <v>8</v>
@@ -2931,7 +2937,7 @@
       <c r="AN24" s="1"/>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A25" s="8"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="1" t="s">
         <v>97</v>
       </c>
@@ -2941,7 +2947,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>18</v>
@@ -2989,7 +2995,7 @@
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
       <c r="AD25" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AE25" s="1" t="s">
         <v>10</v>
@@ -3005,7 +3011,7 @@
       <c r="AN25" s="1"/>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A26" s="8"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="1" t="s">
         <v>96</v>
       </c>
@@ -3015,7 +3021,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>4</v>
+        <v>224</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>26</v>
@@ -3063,7 +3069,7 @@
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
       <c r="AD26" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="AE26" s="1" t="s">
         <v>12</v>
@@ -3122,11 +3128,11 @@
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -3176,47 +3182,47 @@
         <v>57</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="10" t="s">
+      <c r="J29" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="10" t="s">
+      <c r="N29" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
       <c r="Q29" s="2"/>
-      <c r="R29" s="10" t="s">
+      <c r="R29" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S29" s="10"/>
-      <c r="T29" s="10"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
       <c r="U29" s="2"/>
-      <c r="V29" s="10" t="s">
+      <c r="V29" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W29" s="10"/>
-      <c r="X29" s="10"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="7"/>
       <c r="Y29" s="2"/>
-      <c r="Z29" s="10" t="s">
+      <c r="Z29" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA29" s="10"/>
-      <c r="AB29" s="10"/>
+      <c r="AA29" s="7"/>
+      <c r="AB29" s="7"/>
       <c r="AC29" s="2"/>
-      <c r="AD29" s="10" t="s">
+      <c r="AD29" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE29" s="10"/>
-      <c r="AF29" s="10"/>
+      <c r="AE29" s="7"/>
+      <c r="AF29" s="7"/>
       <c r="AG29" s="1"/>
       <c r="AH29" s="1"/>
       <c r="AI29" s="1"/>
@@ -3227,7 +3233,7 @@
       <c r="AN29" s="1"/>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -3319,7 +3325,7 @@
       <c r="AN30" s="1"/>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A31" s="8"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="1" t="s">
         <v>183</v>
       </c>
@@ -3409,7 +3415,7 @@
       <c r="AN31" s="1"/>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A32" s="8"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="1" t="s">
         <v>184</v>
       </c>
@@ -3499,7 +3505,7 @@
       <c r="AN32" s="1"/>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A33" s="8"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="1" t="s">
         <v>185</v>
       </c>
@@ -3589,7 +3595,7 @@
       <c r="AN33" s="1"/>
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A34" s="8"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="1" t="s">
         <v>182</v>
       </c>
@@ -3679,7 +3685,7 @@
       <c r="AN34" s="1"/>
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A35" s="8"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="1" t="s">
         <v>186</v>
       </c>
@@ -3769,7 +3775,7 @@
       <c r="AN35" s="1"/>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A36" s="8"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="1" t="s">
         <v>181</v>
       </c>
@@ -3781,13 +3787,13 @@
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1" t="s">
@@ -3912,58 +3918,58 @@
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="10" t="s">
+      <c r="F38" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
       <c r="I38" s="2"/>
-      <c r="J38" s="10" t="s">
+      <c r="J38" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
       <c r="M38" s="2"/>
-      <c r="N38" s="10" t="s">
+      <c r="N38" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
       <c r="Q38" s="2"/>
-      <c r="R38" s="10" t="s">
+      <c r="R38" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S38" s="10"/>
-      <c r="T38" s="10"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
       <c r="U38" s="2"/>
-      <c r="V38" s="10" t="s">
+      <c r="V38" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W38" s="10"/>
-      <c r="X38" s="10"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="7"/>
       <c r="Y38" s="2"/>
-      <c r="Z38" s="10" t="s">
+      <c r="Z38" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA38" s="10"/>
-      <c r="AB38" s="10"/>
+      <c r="AA38" s="7"/>
+      <c r="AB38" s="7"/>
       <c r="AC38" s="2"/>
-      <c r="AD38" s="10" t="s">
+      <c r="AD38" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE38" s="10"/>
-      <c r="AF38" s="10"/>
+      <c r="AE38" s="7"/>
+      <c r="AF38" s="7"/>
       <c r="AG38" s="2"/>
       <c r="AH38" s="1"/>
       <c r="AI38" s="1"/>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
-      <c r="AL38" s="10"/>
-      <c r="AM38" s="10"/>
-      <c r="AN38" s="10"/>
+      <c r="AL38" s="7"/>
+      <c r="AM38" s="7"/>
+      <c r="AN38" s="7"/>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -4029,7 +4035,7 @@
         <v>48</v>
       </c>
       <c r="AF39" s="1"/>
-      <c r="AG39" s="8"/>
+      <c r="AG39" s="11"/>
       <c r="AH39" s="1"/>
       <c r="AI39" s="1"/>
       <c r="AJ39" s="1"/>
@@ -4039,7 +4045,7 @@
       <c r="AN39" s="1"/>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A40" s="8"/>
+      <c r="A40" s="11"/>
       <c r="B40" s="1" t="s">
         <v>111</v>
       </c>
@@ -4103,7 +4109,7 @@
         <v>31</v>
       </c>
       <c r="AF40" s="1"/>
-      <c r="AG40" s="8"/>
+      <c r="AG40" s="11"/>
       <c r="AH40" s="1"/>
       <c r="AI40" s="1"/>
       <c r="AJ40" s="1"/>
@@ -4113,7 +4119,7 @@
       <c r="AN40" s="1"/>
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A41" s="8"/>
+      <c r="A41" s="11"/>
       <c r="B41" s="1" t="s">
         <v>198</v>
       </c>
@@ -4177,7 +4183,7 @@
         <v>20</v>
       </c>
       <c r="AF41" s="1"/>
-      <c r="AG41" s="8"/>
+      <c r="AG41" s="11"/>
       <c r="AH41" s="1"/>
       <c r="AI41" s="1"/>
       <c r="AJ41" s="1"/>
@@ -4187,7 +4193,7 @@
       <c r="AN41" s="1"/>
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A42" s="8"/>
+      <c r="A42" s="11"/>
       <c r="B42" s="1" t="s">
         <v>199</v>
       </c>
@@ -4251,7 +4257,7 @@
         <v>28</v>
       </c>
       <c r="AF42" s="1"/>
-      <c r="AG42" s="8"/>
+      <c r="AG42" s="11"/>
       <c r="AH42" s="1"/>
       <c r="AI42" s="1"/>
       <c r="AJ42" s="1"/>
@@ -4261,7 +4267,7 @@
       <c r="AN42" s="1"/>
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A43" s="8"/>
+      <c r="A43" s="11"/>
       <c r="B43" s="1" t="s">
         <v>196</v>
       </c>
@@ -4325,7 +4331,7 @@
         <v>9</v>
       </c>
       <c r="AF43" s="1"/>
-      <c r="AG43" s="8"/>
+      <c r="AG43" s="11"/>
       <c r="AH43" s="1"/>
       <c r="AI43" s="1"/>
       <c r="AJ43" s="1"/>
@@ -4335,7 +4341,7 @@
       <c r="AN43" s="1"/>
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A44" s="8"/>
+      <c r="A44" s="11"/>
       <c r="B44" s="1" t="s">
         <v>197</v>
       </c>
@@ -4396,10 +4402,10 @@
         <v>10</v>
       </c>
       <c r="AE44" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AF44" s="1"/>
-      <c r="AG44" s="8"/>
+      <c r="AG44" s="11"/>
       <c r="AH44" s="1"/>
       <c r="AI44" s="1"/>
       <c r="AJ44" s="1"/>
@@ -4409,7 +4415,7 @@
       <c r="AN44" s="1"/>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A45" s="8"/>
+      <c r="A45" s="11"/>
       <c r="B45" s="1" t="s">
         <v>72</v>
       </c>
@@ -4467,13 +4473,13 @@
       <c r="AB45" s="1"/>
       <c r="AC45" s="1"/>
       <c r="AD45" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="AE45" s="1" t="s">
         <v>12</v>
       </c>
       <c r="AF45" s="1"/>
-      <c r="AG45" s="8"/>
+      <c r="AG45" s="11"/>
       <c r="AH45" s="1"/>
       <c r="AI45" s="1"/>
       <c r="AJ45" s="1"/>
@@ -4534,47 +4540,47 @@
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="10" t="s">
+      <c r="F47" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
       <c r="I47" s="2"/>
-      <c r="J47" s="10" t="s">
+      <c r="J47" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K47" s="10"/>
-      <c r="L47" s="10"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
       <c r="M47" s="2"/>
-      <c r="N47" s="10" t="s">
+      <c r="N47" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O47" s="10"/>
-      <c r="P47" s="10"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
       <c r="Q47" s="2"/>
-      <c r="R47" s="10" t="s">
+      <c r="R47" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S47" s="10"/>
-      <c r="T47" s="10"/>
+      <c r="S47" s="7"/>
+      <c r="T47" s="7"/>
       <c r="U47" s="2"/>
-      <c r="V47" s="10" t="s">
+      <c r="V47" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W47" s="10"/>
-      <c r="X47" s="10"/>
+      <c r="W47" s="7"/>
+      <c r="X47" s="7"/>
       <c r="Y47" s="2"/>
-      <c r="Z47" s="10" t="s">
+      <c r="Z47" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA47" s="10"/>
-      <c r="AB47" s="10"/>
+      <c r="AA47" s="7"/>
+      <c r="AB47" s="7"/>
       <c r="AC47" s="2"/>
-      <c r="AD47" s="10" t="s">
+      <c r="AD47" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE47" s="10"/>
-      <c r="AF47" s="10"/>
+      <c r="AE47" s="7"/>
+      <c r="AF47" s="7"/>
       <c r="AG47" s="1"/>
       <c r="AH47" s="1"/>
       <c r="AI47" s="1"/>
@@ -4585,7 +4591,7 @@
       <c r="AN47" s="1"/>
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -4661,7 +4667,7 @@
       <c r="AN48" s="1"/>
     </row>
     <row r="49" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A49" s="8"/>
+      <c r="A49" s="11"/>
       <c r="B49" s="1" t="s">
         <v>200</v>
       </c>
@@ -4735,7 +4741,7 @@
       <c r="AN49" s="1"/>
     </row>
     <row r="50" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A50" s="8"/>
+      <c r="A50" s="11"/>
       <c r="B50" s="1" t="s">
         <v>112</v>
       </c>
@@ -4809,7 +4815,7 @@
       <c r="AN50" s="1"/>
     </row>
     <row r="51" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A51" s="8"/>
+      <c r="A51" s="11"/>
       <c r="B51" s="1" t="s">
         <v>117</v>
       </c>
@@ -4883,7 +4889,7 @@
       <c r="AN51" s="1"/>
     </row>
     <row r="52" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A52" s="8"/>
+      <c r="A52" s="11"/>
       <c r="B52" s="1" t="s">
         <v>118</v>
       </c>
@@ -4957,7 +4963,7 @@
       <c r="AN52" s="1"/>
     </row>
     <row r="53" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A53" s="8"/>
+      <c r="A53" s="11"/>
       <c r="B53" s="1" t="s">
         <v>197</v>
       </c>
@@ -5018,7 +5024,7 @@
         <v>10</v>
       </c>
       <c r="AE53" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AF53" s="1"/>
       <c r="AG53" s="1"/>
@@ -5031,7 +5037,7 @@
       <c r="AN53" s="1"/>
     </row>
     <row r="54" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A54" s="8"/>
+      <c r="A54" s="11"/>
       <c r="B54" s="1" t="s">
         <v>72</v>
       </c>
@@ -5089,7 +5095,7 @@
       <c r="AB54" s="1"/>
       <c r="AC54" s="1"/>
       <c r="AD54" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="AE54" s="1" t="s">
         <v>12</v>
@@ -5160,47 +5166,47 @@
         <v>110</v>
       </c>
       <c r="E56" s="1"/>
-      <c r="F56" s="10" t="s">
+      <c r="F56" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
       <c r="I56" s="2"/>
-      <c r="J56" s="10" t="s">
+      <c r="J56" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K56" s="10"/>
-      <c r="L56" s="10"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
       <c r="M56" s="2"/>
-      <c r="N56" s="10" t="s">
+      <c r="N56" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O56" s="10"/>
-      <c r="P56" s="10"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="7"/>
       <c r="Q56" s="2"/>
-      <c r="R56" s="10" t="s">
+      <c r="R56" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S56" s="10"/>
-      <c r="T56" s="10"/>
+      <c r="S56" s="7"/>
+      <c r="T56" s="7"/>
       <c r="U56" s="2"/>
-      <c r="V56" s="10" t="s">
+      <c r="V56" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W56" s="10"/>
-      <c r="X56" s="10"/>
+      <c r="W56" s="7"/>
+      <c r="X56" s="7"/>
       <c r="Y56" s="2"/>
-      <c r="Z56" s="10" t="s">
+      <c r="Z56" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA56" s="10"/>
-      <c r="AB56" s="10"/>
+      <c r="AA56" s="7"/>
+      <c r="AB56" s="7"/>
       <c r="AC56" s="2"/>
-      <c r="AD56" s="10" t="s">
+      <c r="AD56" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE56" s="10"/>
-      <c r="AF56" s="10"/>
+      <c r="AE56" s="7"/>
+      <c r="AF56" s="7"/>
       <c r="AG56" s="1"/>
       <c r="AH56" s="1"/>
       <c r="AI56" s="1"/>
@@ -5211,7 +5217,7 @@
       <c r="AN56" s="1"/>
     </row>
     <row r="57" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -5303,7 +5309,7 @@
       <c r="AN57" s="1"/>
     </row>
     <row r="58" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A58" s="8"/>
+      <c r="A58" s="11"/>
       <c r="B58" s="1" t="s">
         <v>115</v>
       </c>
@@ -5393,7 +5399,7 @@
       <c r="AN58" s="1"/>
     </row>
     <row r="59" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A59" s="8"/>
+      <c r="A59" s="11"/>
       <c r="B59" s="1" t="s">
         <v>116</v>
       </c>
@@ -5483,7 +5489,7 @@
       <c r="AN59" s="1"/>
     </row>
     <row r="60" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A60" s="8"/>
+      <c r="A60" s="11"/>
       <c r="B60" s="1" t="s">
         <v>113</v>
       </c>
@@ -5573,7 +5579,7 @@
       <c r="AN60" s="1"/>
     </row>
     <row r="61" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A61" s="8"/>
+      <c r="A61" s="11"/>
       <c r="B61" s="1" t="s">
         <v>114</v>
       </c>
@@ -5663,7 +5669,7 @@
       <c r="AN61" s="1"/>
     </row>
     <row r="62" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A62" s="8"/>
+      <c r="A62" s="11"/>
       <c r="B62" s="1" t="s">
         <v>203</v>
       </c>
@@ -5753,7 +5759,7 @@
       <c r="AN62" s="1"/>
     </row>
     <row r="63" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A63" s="8"/>
+      <c r="A63" s="11"/>
       <c r="B63" s="1" t="s">
         <v>102</v>
       </c>
@@ -5825,7 +5831,7 @@
       </c>
       <c r="AC63" s="1"/>
       <c r="AD63" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="AE63" s="1" t="s">
         <v>12</v>
@@ -5896,47 +5902,47 @@
         <v>201</v>
       </c>
       <c r="E65" s="1"/>
-      <c r="F65" s="10" t="s">
+      <c r="F65" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G65" s="10"/>
-      <c r="H65" s="10"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
       <c r="I65" s="2"/>
-      <c r="J65" s="10" t="s">
+      <c r="J65" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K65" s="10"/>
-      <c r="L65" s="10"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
       <c r="M65" s="2"/>
-      <c r="N65" s="10" t="s">
+      <c r="N65" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O65" s="10"/>
-      <c r="P65" s="10"/>
+      <c r="O65" s="7"/>
+      <c r="P65" s="7"/>
       <c r="Q65" s="2"/>
-      <c r="R65" s="10" t="s">
+      <c r="R65" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S65" s="10"/>
-      <c r="T65" s="10"/>
+      <c r="S65" s="7"/>
+      <c r="T65" s="7"/>
       <c r="U65" s="2"/>
-      <c r="V65" s="10" t="s">
+      <c r="V65" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W65" s="10"/>
-      <c r="X65" s="10"/>
+      <c r="W65" s="7"/>
+      <c r="X65" s="7"/>
       <c r="Y65" s="2"/>
-      <c r="Z65" s="10" t="s">
+      <c r="Z65" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA65" s="10"/>
-      <c r="AB65" s="10"/>
+      <c r="AA65" s="7"/>
+      <c r="AB65" s="7"/>
       <c r="AC65" s="2"/>
-      <c r="AD65" s="10" t="s">
+      <c r="AD65" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE65" s="10"/>
-      <c r="AF65" s="10"/>
+      <c r="AE65" s="7"/>
+      <c r="AF65" s="7"/>
       <c r="AG65" s="1"/>
       <c r="AH65" s="1"/>
       <c r="AI65" s="1"/>
@@ -5947,7 +5953,7 @@
       <c r="AN65" s="1"/>
     </row>
     <row r="66" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A66" s="8" t="s">
+      <c r="A66" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -6039,7 +6045,7 @@
       <c r="AN66" s="1"/>
     </row>
     <row r="67" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A67" s="8"/>
+      <c r="A67" s="11"/>
       <c r="B67" s="1" t="s">
         <v>126</v>
       </c>
@@ -6129,7 +6135,7 @@
       <c r="AN67" s="1"/>
     </row>
     <row r="68" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A68" s="8"/>
+      <c r="A68" s="11"/>
       <c r="B68" s="1" t="s">
         <v>206</v>
       </c>
@@ -6219,7 +6225,7 @@
       <c r="AN68" s="1"/>
     </row>
     <row r="69" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A69" s="8"/>
+      <c r="A69" s="11"/>
       <c r="B69" s="1" t="s">
         <v>204</v>
       </c>
@@ -6309,7 +6315,7 @@
       <c r="AN69" s="1"/>
     </row>
     <row r="70" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A70" s="8"/>
+      <c r="A70" s="11"/>
       <c r="B70" s="1" t="s">
         <v>123</v>
       </c>
@@ -6399,7 +6405,7 @@
       <c r="AN70" s="1"/>
     </row>
     <row r="71" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A71" s="8"/>
+      <c r="A71" s="11"/>
       <c r="B71" s="1" t="s">
         <v>124</v>
       </c>
@@ -6489,7 +6495,7 @@
       <c r="AN71" s="1"/>
     </row>
     <row r="72" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A72" s="8"/>
+      <c r="A72" s="11"/>
       <c r="B72" s="1" t="s">
         <v>125</v>
       </c>
@@ -6561,7 +6567,7 @@
       </c>
       <c r="AC72" s="1"/>
       <c r="AD72" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="AE72" s="1" t="s">
         <v>12</v>
@@ -6622,9 +6628,9 @@
     </row>
     <row r="74" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -6670,47 +6676,47 @@
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="10" t="s">
+      <c r="F75" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G75" s="10"/>
-      <c r="H75" s="10"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
       <c r="I75" s="2"/>
-      <c r="J75" s="10" t="s">
+      <c r="J75" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K75" s="10"/>
-      <c r="L75" s="10"/>
+      <c r="K75" s="7"/>
+      <c r="L75" s="7"/>
       <c r="M75" s="2"/>
-      <c r="N75" s="10" t="s">
+      <c r="N75" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O75" s="10"/>
-      <c r="P75" s="10"/>
+      <c r="O75" s="7"/>
+      <c r="P75" s="7"/>
       <c r="Q75" s="2"/>
-      <c r="R75" s="10" t="s">
+      <c r="R75" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S75" s="10"/>
-      <c r="T75" s="10"/>
+      <c r="S75" s="7"/>
+      <c r="T75" s="7"/>
       <c r="U75" s="2"/>
-      <c r="V75" s="10" t="s">
+      <c r="V75" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W75" s="10"/>
-      <c r="X75" s="10"/>
+      <c r="W75" s="7"/>
+      <c r="X75" s="7"/>
       <c r="Y75" s="2"/>
-      <c r="Z75" s="10" t="s">
+      <c r="Z75" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA75" s="10"/>
-      <c r="AB75" s="10"/>
+      <c r="AA75" s="7"/>
+      <c r="AB75" s="7"/>
       <c r="AC75" s="2"/>
-      <c r="AD75" s="10" t="s">
+      <c r="AD75" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE75" s="10"/>
-      <c r="AF75" s="10"/>
+      <c r="AE75" s="7"/>
+      <c r="AF75" s="7"/>
       <c r="AG75" s="1"/>
       <c r="AH75" s="1"/>
       <c r="AI75" s="1"/>
@@ -6721,7 +6727,7 @@
       <c r="AN75" s="1"/>
     </row>
     <row r="76" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A76" s="8" t="s">
+      <c r="A76" s="11" t="s">
         <v>50</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -6813,7 +6819,7 @@
       <c r="AN76" s="1"/>
     </row>
     <row r="77" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A77" s="8"/>
+      <c r="A77" s="11"/>
       <c r="B77" s="1" t="s">
         <v>53</v>
       </c>
@@ -6903,7 +6909,7 @@
       <c r="AN77" s="1"/>
     </row>
     <row r="78" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A78" s="8"/>
+      <c r="A78" s="11"/>
       <c r="B78" s="1" t="s">
         <v>40</v>
       </c>
@@ -6975,7 +6981,7 @@
       </c>
       <c r="AC78" s="1"/>
       <c r="AD78" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="AE78" s="1" t="s">
         <v>20</v>
@@ -6993,7 +6999,7 @@
       <c r="AN78" s="1"/>
     </row>
     <row r="79" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A79" s="8"/>
+      <c r="A79" s="11"/>
       <c r="B79" s="1" t="s">
         <v>34</v>
       </c>
@@ -7035,7 +7041,7 @@
       </c>
       <c r="Q79" s="1"/>
       <c r="R79" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="S79" s="1" t="s">
         <v>10</v>
@@ -7045,7 +7051,7 @@
       </c>
       <c r="U79" s="1"/>
       <c r="V79" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="W79" s="1" t="s">
         <v>9</v>
@@ -7055,7 +7061,7 @@
       </c>
       <c r="Y79" s="1"/>
       <c r="Z79" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="AA79" s="1" t="s">
         <v>8</v>
@@ -7065,7 +7071,7 @@
       </c>
       <c r="AC79" s="1"/>
       <c r="AD79" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AE79" s="1" t="s">
         <v>28</v>
@@ -7083,7 +7089,7 @@
       <c r="AN79" s="1"/>
     </row>
     <row r="80" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A80" s="8"/>
+      <c r="A80" s="11"/>
       <c r="B80" s="1" t="s">
         <v>35</v>
       </c>
@@ -7145,7 +7151,7 @@
       </c>
       <c r="Y80" s="1"/>
       <c r="Z80" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AA80" s="1" t="s">
         <v>10</v>
@@ -7155,7 +7161,7 @@
       </c>
       <c r="AC80" s="1"/>
       <c r="AD80" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AE80" s="1" t="s">
         <v>9</v>
@@ -7173,7 +7179,7 @@
       <c r="AN80" s="1"/>
     </row>
     <row r="81" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A81" s="8"/>
+      <c r="A81" s="11"/>
       <c r="B81" s="1" t="s">
         <v>11</v>
       </c>
@@ -7191,7 +7197,7 @@
         <v>14</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="I81" s="1"/>
       <c r="J81" s="1" t="s">
@@ -7235,7 +7241,7 @@
       </c>
       <c r="Y81" s="1"/>
       <c r="Z81" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AA81" s="1" t="s">
         <v>12</v>
@@ -7245,7 +7251,7 @@
       </c>
       <c r="AC81" s="1"/>
       <c r="AD81" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AE81" s="1" t="s">
         <v>11</v>
@@ -7263,7 +7269,7 @@
       <c r="AN81" s="1"/>
     </row>
     <row r="82" spans="1:40" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="8"/>
+      <c r="A82" s="11"/>
       <c r="B82" s="1" t="s">
         <v>12</v>
       </c>
@@ -7281,7 +7287,7 @@
         <v>6</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="I82" s="1"/>
       <c r="J82" s="1" t="s">
@@ -7325,7 +7331,7 @@
       </c>
       <c r="Y82" s="1"/>
       <c r="Z82" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="AA82" s="1" t="s">
         <v>22</v>
@@ -7341,7 +7347,7 @@
         <v>12</v>
       </c>
       <c r="AF82" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="AG82" s="1"/>
       <c r="AH82" s="1"/>
@@ -7396,9 +7402,9 @@
     </row>
     <row r="84" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
-      <c r="B84" s="7"/>
-      <c r="C84" s="7"/>
-      <c r="D84" s="7"/>
+      <c r="B84" s="12"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
@@ -7446,47 +7452,47 @@
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
-      <c r="F85" s="10" t="s">
+      <c r="F85" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G85" s="10"/>
-      <c r="H85" s="10"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
       <c r="I85" s="2"/>
-      <c r="J85" s="10" t="s">
+      <c r="J85" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K85" s="10"/>
-      <c r="L85" s="10"/>
+      <c r="K85" s="7"/>
+      <c r="L85" s="7"/>
       <c r="M85" s="2"/>
-      <c r="N85" s="10" t="s">
+      <c r="N85" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O85" s="10"/>
-      <c r="P85" s="10"/>
+      <c r="O85" s="7"/>
+      <c r="P85" s="7"/>
       <c r="Q85" s="2"/>
-      <c r="R85" s="10" t="s">
+      <c r="R85" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S85" s="10"/>
-      <c r="T85" s="10"/>
+      <c r="S85" s="7"/>
+      <c r="T85" s="7"/>
       <c r="U85" s="2"/>
-      <c r="V85" s="10" t="s">
+      <c r="V85" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W85" s="10"/>
-      <c r="X85" s="10"/>
+      <c r="W85" s="7"/>
+      <c r="X85" s="7"/>
       <c r="Y85" s="2"/>
-      <c r="Z85" s="10" t="s">
+      <c r="Z85" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA85" s="10"/>
-      <c r="AB85" s="10"/>
+      <c r="AA85" s="7"/>
+      <c r="AB85" s="7"/>
       <c r="AC85" s="2"/>
-      <c r="AD85" s="10" t="s">
+      <c r="AD85" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE85" s="10"/>
-      <c r="AF85" s="10"/>
+      <c r="AE85" s="7"/>
+      <c r="AF85" s="7"/>
       <c r="AG85" s="1"/>
       <c r="AH85" s="1"/>
       <c r="AI85" s="1"/>
@@ -7497,7 +7503,7 @@
       <c r="AN85" s="1"/>
     </row>
     <row r="86" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A86" s="8" t="s">
+      <c r="A86" s="11" t="s">
         <v>55</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -7589,7 +7595,7 @@
       <c r="AN86" s="1"/>
     </row>
     <row r="87" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A87" s="8"/>
+      <c r="A87" s="11"/>
       <c r="B87" s="1" t="s">
         <v>218</v>
       </c>
@@ -7679,7 +7685,7 @@
       <c r="AN87" s="1"/>
     </row>
     <row r="88" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A88" s="8"/>
+      <c r="A88" s="11"/>
       <c r="B88" s="1" t="s">
         <v>34</v>
       </c>
@@ -7769,7 +7775,7 @@
       <c r="AN88" s="1"/>
     </row>
     <row r="89" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A89" s="8"/>
+      <c r="A89" s="11"/>
       <c r="B89" s="1" t="s">
         <v>9</v>
       </c>
@@ -7859,7 +7865,7 @@
       <c r="AN89" s="1"/>
     </row>
     <row r="90" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A90" s="8"/>
+      <c r="A90" s="11"/>
       <c r="B90" s="1" t="s">
         <v>10</v>
       </c>
@@ -7871,7 +7877,7 @@
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>14</v>
@@ -7949,7 +7955,7 @@
       <c r="AN90" s="1"/>
     </row>
     <row r="91" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A91" s="8"/>
+      <c r="A91" s="11"/>
       <c r="B91" s="1" t="s">
         <v>11</v>
       </c>
@@ -7961,7 +7967,7 @@
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>6</v>
@@ -8039,7 +8045,7 @@
       <c r="AN91" s="1"/>
     </row>
     <row r="92" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A92" s="8"/>
+      <c r="A92" s="11"/>
       <c r="B92" s="1" t="s">
         <v>12</v>
       </c>
@@ -8051,7 +8057,7 @@
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>15</v>
@@ -8178,29 +8184,29 @@
         <v>222</v>
       </c>
       <c r="E94" s="1"/>
-      <c r="F94" s="10" t="s">
+      <c r="F94" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="G94" s="10"/>
-      <c r="H94" s="10"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
       <c r="I94" s="2"/>
-      <c r="J94" s="10" t="s">
+      <c r="J94" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K94" s="10"/>
-      <c r="L94" s="10"/>
+      <c r="K94" s="7"/>
+      <c r="L94" s="7"/>
       <c r="M94" s="2"/>
-      <c r="N94" s="10" t="s">
+      <c r="N94" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="O94" s="10"/>
-      <c r="P94" s="10"/>
+      <c r="O94" s="7"/>
+      <c r="P94" s="7"/>
       <c r="Q94" s="2"/>
-      <c r="R94" s="10" t="s">
+      <c r="R94" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="S94" s="10"/>
-      <c r="T94" s="10"/>
+      <c r="S94" s="7"/>
+      <c r="T94" s="7"/>
       <c r="U94" s="1"/>
       <c r="V94" s="1"/>
       <c r="W94" s="1"/>
@@ -8223,7 +8229,7 @@
       <c r="AN94" s="1"/>
     </row>
     <row r="95" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="9" t="s">
+      <c r="A95" s="8" t="s">
         <v>138</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -8297,7 +8303,7 @@
       <c r="AN95" s="1"/>
     </row>
     <row r="96" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="9"/>
+      <c r="A96" s="8"/>
       <c r="B96" s="1" t="s">
         <v>145</v>
       </c>
@@ -8369,7 +8375,7 @@
       <c r="AN96" s="1"/>
     </row>
     <row r="97" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="9"/>
+      <c r="A97" s="8"/>
       <c r="B97" s="1" t="s">
         <v>146</v>
       </c>
@@ -8441,7 +8447,7 @@
       <c r="AN97" s="1"/>
     </row>
     <row r="98" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="9"/>
+      <c r="A98" s="8"/>
       <c r="B98" s="1" t="s">
         <v>147</v>
       </c>
@@ -8513,7 +8519,7 @@
       <c r="AN98" s="1"/>
     </row>
     <row r="99" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="9"/>
+      <c r="A99" s="8"/>
       <c r="B99" s="1" t="s">
         <v>148</v>
       </c>
@@ -8585,7 +8591,7 @@
       <c r="AN99" s="1"/>
     </row>
     <row r="100" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="9"/>
+      <c r="A100" s="8"/>
       <c r="B100" s="1" t="s">
         <v>149</v>
       </c>
@@ -8657,7 +8663,7 @@
       <c r="AN100" s="1"/>
     </row>
     <row r="101" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="9"/>
+      <c r="A101" s="8"/>
       <c r="B101" s="1" t="s">
         <v>150</v>
       </c>
@@ -8776,29 +8782,29 @@
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
-      <c r="F103" s="10" t="s">
+      <c r="F103" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="G103" s="10"/>
-      <c r="H103" s="10"/>
+      <c r="G103" s="7"/>
+      <c r="H103" s="7"/>
       <c r="I103" s="2"/>
-      <c r="J103" s="10" t="s">
+      <c r="J103" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K103" s="10"/>
-      <c r="L103" s="10"/>
+      <c r="K103" s="7"/>
+      <c r="L103" s="7"/>
       <c r="M103" s="2"/>
-      <c r="N103" s="10" t="s">
+      <c r="N103" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="O103" s="10"/>
-      <c r="P103" s="10"/>
+      <c r="O103" s="7"/>
+      <c r="P103" s="7"/>
       <c r="Q103" s="2"/>
-      <c r="R103" s="10" t="s">
+      <c r="R103" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="S103" s="10"/>
-      <c r="T103" s="10"/>
+      <c r="S103" s="7"/>
+      <c r="T103" s="7"/>
       <c r="U103" s="1"/>
       <c r="V103" s="1"/>
       <c r="W103" s="1"/>
@@ -8821,7 +8827,7 @@
       <c r="AN103" s="1"/>
     </row>
     <row r="104" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="9" t="s">
+      <c r="A104" s="8" t="s">
         <v>162</v>
       </c>
       <c r="B104" s="1" t="s">
@@ -8887,7 +8893,7 @@
       <c r="AN104" s="1"/>
     </row>
     <row r="105" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="9"/>
+      <c r="A105" s="8"/>
       <c r="B105" s="1" t="s">
         <v>12</v>
       </c>
@@ -8959,7 +8965,7 @@
       <c r="AN105" s="1"/>
     </row>
     <row r="106" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="9"/>
+      <c r="A106" s="8"/>
       <c r="B106" s="1" t="s">
         <v>102</v>
       </c>
@@ -9031,7 +9037,7 @@
       <c r="AN106" s="1"/>
     </row>
     <row r="107" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="9"/>
+      <c r="A107" s="8"/>
       <c r="B107" s="1" t="s">
         <v>167</v>
       </c>
@@ -9103,7 +9109,7 @@
       <c r="AN107" s="1"/>
     </row>
     <row r="108" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="9"/>
+      <c r="A108" s="8"/>
       <c r="B108" s="1" t="s">
         <v>166</v>
       </c>
@@ -9175,7 +9181,7 @@
       <c r="AN108" s="1"/>
     </row>
     <row r="109" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="9"/>
+      <c r="A109" s="8"/>
       <c r="B109" s="1" t="s">
         <v>164</v>
       </c>
@@ -9247,7 +9253,7 @@
       <c r="AN109" s="1"/>
     </row>
     <row r="110" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="9"/>
+      <c r="A110" s="8"/>
       <c r="B110" s="1" t="s">
         <v>165</v>
       </c>
@@ -9319,7 +9325,7 @@
       <c r="AN110" s="1"/>
     </row>
     <row r="112" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A112" s="9" t="s">
+      <c r="A112" s="8" t="s">
         <v>74</v>
       </c>
       <c r="B112" s="1"/>
@@ -9338,13 +9344,13 @@
       <c r="G112" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H112" s="12" t="s">
+      <c r="H112" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="I112" s="12"/>
+      <c r="I112" s="9"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A113" s="9"/>
+      <c r="A113" s="8"/>
       <c r="B113" s="1" t="s">
         <v>13</v>
       </c>
@@ -9363,11 +9369,11 @@
       <c r="G113" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H113" s="12"/>
-      <c r="I113" s="12"/>
+      <c r="H113" s="9"/>
+      <c r="I113" s="9"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A114" s="9"/>
+      <c r="A114" s="8"/>
       <c r="B114" s="1" t="s">
         <v>17</v>
       </c>
@@ -9386,11 +9392,11 @@
       <c r="G114" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H114" s="12"/>
-      <c r="I114" s="12"/>
+      <c r="H114" s="9"/>
+      <c r="I114" s="9"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A115" s="9"/>
+      <c r="A115" s="8"/>
       <c r="B115" s="1" t="s">
         <v>21</v>
       </c>
@@ -9409,11 +9415,11 @@
       <c r="G115" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H115" s="12"/>
-      <c r="I115" s="12"/>
+      <c r="H115" s="9"/>
+      <c r="I115" s="9"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A116" s="9"/>
+      <c r="A116" s="8"/>
       <c r="B116" s="1" t="s">
         <v>23</v>
       </c>
@@ -9432,11 +9438,11 @@
       <c r="G116" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H116" s="12"/>
-      <c r="I116" s="12"/>
+      <c r="H116" s="9"/>
+      <c r="I116" s="9"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A117" s="9"/>
+      <c r="A117" s="8"/>
       <c r="B117" s="1" t="s">
         <v>25</v>
       </c>
@@ -9455,11 +9461,11 @@
       <c r="G117" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H117" s="12"/>
-      <c r="I117" s="12"/>
+      <c r="H117" s="9"/>
+      <c r="I117" s="9"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A118" s="9"/>
+      <c r="A118" s="8"/>
       <c r="B118" s="1" t="s">
         <v>30</v>
       </c>
@@ -9478,11 +9484,11 @@
       <c r="G118" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H118" s="12"/>
-      <c r="I118" s="12"/>
+      <c r="H118" s="9"/>
+      <c r="I118" s="9"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A119" s="9"/>
+      <c r="A119" s="8"/>
       <c r="B119" s="1" t="s">
         <v>75</v>
       </c>
@@ -9501,32 +9507,74 @@
       <c r="G119" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H119" s="12"/>
-      <c r="I119" s="12"/>
+      <c r="H119" s="9"/>
+      <c r="I119" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="99">
-    <mergeCell ref="R94:T94"/>
-    <mergeCell ref="A95:A101"/>
-    <mergeCell ref="F103:H103"/>
-    <mergeCell ref="J103:L103"/>
-    <mergeCell ref="N103:P103"/>
-    <mergeCell ref="R103:T103"/>
-    <mergeCell ref="A112:A119"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="J94:L94"/>
-    <mergeCell ref="N94:P94"/>
-    <mergeCell ref="A104:A110"/>
-    <mergeCell ref="H112:I119"/>
-    <mergeCell ref="F1:AF1"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="A86:A92"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="A57:A63"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="Z75:AB75"/>
+    <mergeCell ref="AD75:AF75"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="N85:P85"/>
+    <mergeCell ref="R85:T85"/>
+    <mergeCell ref="V85:X85"/>
+    <mergeCell ref="Z85:AB85"/>
+    <mergeCell ref="AD85:AF85"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="J75:L75"/>
+    <mergeCell ref="N75:P75"/>
+    <mergeCell ref="R75:T75"/>
+    <mergeCell ref="V75:X75"/>
+    <mergeCell ref="Z56:AB56"/>
+    <mergeCell ref="AD56:AF56"/>
+    <mergeCell ref="V65:X65"/>
+    <mergeCell ref="Z65:AB65"/>
+    <mergeCell ref="AD65:AF65"/>
+    <mergeCell ref="V56:X56"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="J65:L65"/>
+    <mergeCell ref="N65:P65"/>
+    <mergeCell ref="R65:T65"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="J56:L56"/>
+    <mergeCell ref="N56:P56"/>
+    <mergeCell ref="R56:T56"/>
+    <mergeCell ref="AL38:AN38"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="AG39:AG45"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="J47:L47"/>
+    <mergeCell ref="N47:P47"/>
+    <mergeCell ref="R47:T47"/>
+    <mergeCell ref="V47:X47"/>
+    <mergeCell ref="Z47:AB47"/>
+    <mergeCell ref="AD47:AF47"/>
+    <mergeCell ref="Z29:AB29"/>
+    <mergeCell ref="AD29:AF29"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="N38:P38"/>
+    <mergeCell ref="R38:T38"/>
+    <mergeCell ref="V38:X38"/>
+    <mergeCell ref="Z38:AB38"/>
+    <mergeCell ref="AD38:AF38"/>
+    <mergeCell ref="V29:X29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="R29:T29"/>
     <mergeCell ref="AD11:AF11"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="F19:H19"/>
@@ -9542,69 +9590,27 @@
     <mergeCell ref="R11:T11"/>
     <mergeCell ref="V11:X11"/>
     <mergeCell ref="Z11:AB11"/>
-    <mergeCell ref="Z29:AB29"/>
-    <mergeCell ref="AD29:AF29"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="N38:P38"/>
-    <mergeCell ref="R38:T38"/>
-    <mergeCell ref="V38:X38"/>
-    <mergeCell ref="Z38:AB38"/>
-    <mergeCell ref="AD38:AF38"/>
-    <mergeCell ref="V29:X29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="AL38:AN38"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="AG39:AG45"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="J47:L47"/>
-    <mergeCell ref="N47:P47"/>
-    <mergeCell ref="R47:T47"/>
-    <mergeCell ref="V47:X47"/>
-    <mergeCell ref="Z47:AB47"/>
-    <mergeCell ref="AD47:AF47"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="J65:L65"/>
-    <mergeCell ref="N65:P65"/>
-    <mergeCell ref="R65:T65"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="J56:L56"/>
-    <mergeCell ref="N56:P56"/>
-    <mergeCell ref="R56:T56"/>
-    <mergeCell ref="Z56:AB56"/>
-    <mergeCell ref="AD56:AF56"/>
-    <mergeCell ref="V65:X65"/>
-    <mergeCell ref="Z65:AB65"/>
-    <mergeCell ref="AD65:AF65"/>
-    <mergeCell ref="V56:X56"/>
-    <mergeCell ref="Z75:AB75"/>
-    <mergeCell ref="AD75:AF75"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="N85:P85"/>
-    <mergeCell ref="R85:T85"/>
-    <mergeCell ref="V85:X85"/>
-    <mergeCell ref="Z85:AB85"/>
-    <mergeCell ref="AD85:AF85"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="J75:L75"/>
-    <mergeCell ref="N75:P75"/>
-    <mergeCell ref="R75:T75"/>
-    <mergeCell ref="V75:X75"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="A86:A92"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A66:A72"/>
-    <mergeCell ref="A57:A63"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F1:AF1"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="A112:A119"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="J94:L94"/>
+    <mergeCell ref="N94:P94"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="H112:I119"/>
+    <mergeCell ref="R94:T94"/>
+    <mergeCell ref="A95:A101"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="J103:L103"/>
+    <mergeCell ref="N103:P103"/>
+    <mergeCell ref="R103:T103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated logic & added DataFrame columns
</commit_message>
<xml_diff>
--- a/Files/Progression Regression Logic.xlsx
+++ b/Files/Progression Regression Logic.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethpe\OneDrive\Documents\Git\madden22stats\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40f61192ff96ff75/Documents/Git/madden22stats/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4525A2FD-8FCF-4C1C-8965-B5B6FED6E457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{BFDC62EA-92D5-4D5A-8117-4E2823A76894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{54C2E4B7-FBFF-4F69-A3A4-847FA497B9AB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="223">
   <si>
     <t>Yards</t>
   </si>
@@ -424,9 +424,6 @@
   </si>
   <si>
     <t>0-0.25</t>
-  </si>
-  <si>
-    <t>TOs (5 Columns)</t>
   </si>
   <si>
     <t>PD/game</t>
@@ -798,19 +795,19 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1131,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39242688-C415-4EFE-B0A8-90C7EAED6EC3}">
   <dimension ref="A1:AN119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I121" sqref="I121"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1145,42 +1142,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="26" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="9"/>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="9"/>
-      <c r="AF1" s="9"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
@@ -1191,7 +1188,7 @@
       <c r="AN1" s="1"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1202,47 +1199,47 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="7" t="s">
+      <c r="V2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
       <c r="Y2" s="2"/>
-      <c r="Z2" s="7" t="s">
+      <c r="Z2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
       <c r="AC2" s="2"/>
-      <c r="AD2" s="7" t="s">
+      <c r="AD2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
@@ -1253,7 +1250,7 @@
       <c r="AN2" s="2"/>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>65</v>
       </c>
@@ -1343,7 +1340,7 @@
       <c r="AN3" s="1"/>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A4" s="10"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>60</v>
       </c>
@@ -1433,7 +1430,7 @@
       <c r="AN4" s="1"/>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A5" s="10"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>61</v>
       </c>
@@ -1523,7 +1520,7 @@
       <c r="AN5" s="1"/>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="1" t="s">
         <v>62</v>
       </c>
@@ -1613,7 +1610,7 @@
       <c r="AN6" s="1"/>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A7" s="10"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1" t="s">
         <v>63</v>
       </c>
@@ -1703,7 +1700,7 @@
       <c r="AN7" s="1"/>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A8" s="10"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>64</v>
       </c>
@@ -1793,7 +1790,7 @@
       <c r="AN8" s="1"/>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="1" t="s">
         <v>54</v>
       </c>
@@ -1934,47 +1931,47 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="7" t="s">
+      <c r="N11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
       <c r="Q11" s="2"/>
-      <c r="R11" s="7" t="s">
+      <c r="R11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
       <c r="U11" s="2"/>
-      <c r="V11" s="7" t="s">
+      <c r="V11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
       <c r="Y11" s="2"/>
-      <c r="Z11" s="7" t="s">
+      <c r="Z11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="7"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="10"/>
       <c r="AC11" s="2"/>
-      <c r="AD11" s="7" t="s">
+      <c r="AD11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE11" s="7"/>
-      <c r="AF11" s="7"/>
+      <c r="AE11" s="10"/>
+      <c r="AF11" s="10"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
@@ -1985,7 +1982,7 @@
       <c r="AN11" s="2"/>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2061,7 +2058,7 @@
       <c r="AN12" s="1"/>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A13" s="10"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
         <v>82</v>
       </c>
@@ -2135,7 +2132,7 @@
       <c r="AN13" s="1"/>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="1" t="s">
         <v>83</v>
       </c>
@@ -2209,7 +2206,7 @@
       <c r="AN14" s="1"/>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="1" t="s">
         <v>84</v>
       </c>
@@ -2283,7 +2280,7 @@
       <c r="AN15" s="1"/>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="1" t="s">
         <v>85</v>
       </c>
@@ -2357,7 +2354,7 @@
       <c r="AN16" s="1"/>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="1" t="s">
         <v>92</v>
       </c>
@@ -2431,7 +2428,7 @@
       <c r="AN17" s="1"/>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A18" s="10"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="1" t="s">
         <v>93</v>
       </c>
@@ -2510,47 +2507,47 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="7" t="s">
+      <c r="J19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="7" t="s">
+      <c r="N19" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
       <c r="Q19" s="2"/>
-      <c r="R19" s="7" t="s">
+      <c r="R19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
       <c r="U19" s="2"/>
-      <c r="V19" s="7" t="s">
+      <c r="V19" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
       <c r="Y19" s="2"/>
-      <c r="Z19" s="7" t="s">
+      <c r="Z19" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA19" s="7"/>
-      <c r="AB19" s="7"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="10"/>
       <c r="AC19" s="2"/>
-      <c r="AD19" s="7" t="s">
+      <c r="AD19" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE19" s="7"/>
-      <c r="AF19" s="7"/>
+      <c r="AE19" s="10"/>
+      <c r="AF19" s="10"/>
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
@@ -2561,7 +2558,7 @@
       <c r="AN19" s="1"/>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2637,7 +2634,7 @@
       <c r="AN20" s="1"/>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A21" s="10"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="1" t="s">
         <v>94</v>
       </c>
@@ -2711,7 +2708,7 @@
       <c r="AN21" s="1"/>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A22" s="10"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="1" t="s">
         <v>95</v>
       </c>
@@ -2785,7 +2782,7 @@
       <c r="AN22" s="1"/>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A23" s="10"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="1" t="s">
         <v>99</v>
       </c>
@@ -2859,7 +2856,7 @@
       <c r="AN23" s="1"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A24" s="10"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="1" t="s">
         <v>98</v>
       </c>
@@ -2933,7 +2930,7 @@
       <c r="AN24" s="1"/>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A25" s="10"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="1" t="s">
         <v>97</v>
       </c>
@@ -3007,7 +3004,7 @@
       <c r="AN25" s="1"/>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A26" s="10"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="1" t="s">
         <v>96</v>
       </c>
@@ -3124,11 +3121,11 @@
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -3178,47 +3175,47 @@
         <v>57</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="7" t="s">
+      <c r="J29" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="7" t="s">
+      <c r="N29" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
       <c r="Q29" s="2"/>
-      <c r="R29" s="7" t="s">
+      <c r="R29" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
       <c r="U29" s="2"/>
-      <c r="V29" s="7" t="s">
+      <c r="V29" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W29" s="7"/>
-      <c r="X29" s="7"/>
+      <c r="W29" s="10"/>
+      <c r="X29" s="10"/>
       <c r="Y29" s="2"/>
-      <c r="Z29" s="7" t="s">
+      <c r="Z29" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA29" s="7"/>
-      <c r="AB29" s="7"/>
+      <c r="AA29" s="10"/>
+      <c r="AB29" s="10"/>
       <c r="AC29" s="2"/>
-      <c r="AD29" s="7" t="s">
+      <c r="AD29" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE29" s="7"/>
-      <c r="AF29" s="7"/>
+      <c r="AE29" s="10"/>
+      <c r="AF29" s="10"/>
       <c r="AG29" s="1"/>
       <c r="AH29" s="1"/>
       <c r="AI29" s="1"/>
@@ -3229,17 +3226,17 @@
       <c r="AN29" s="1"/>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
@@ -3321,15 +3318,15 @@
       <c r="AN30" s="1"/>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A31" s="10"/>
+      <c r="A31" s="8"/>
       <c r="B31" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
@@ -3411,15 +3408,15 @@
       <c r="AN31" s="1"/>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A32" s="10"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
@@ -3501,15 +3498,15 @@
       <c r="AN32" s="1"/>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A33" s="10"/>
+      <c r="A33" s="8"/>
       <c r="B33" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
@@ -3591,15 +3588,15 @@
       <c r="AN33" s="1"/>
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A34" s="10"/>
+      <c r="A34" s="8"/>
       <c r="B34" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
@@ -3681,15 +3678,15 @@
       <c r="AN34" s="1"/>
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A35" s="10"/>
+      <c r="A35" s="8"/>
       <c r="B35" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
@@ -3771,15 +3768,15 @@
       <c r="AN35" s="1"/>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A36" s="10"/>
+      <c r="A36" s="8"/>
       <c r="B36" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
@@ -3910,69 +3907,69 @@
         <v>110</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
       <c r="I38" s="2"/>
-      <c r="J38" s="7" t="s">
+      <c r="J38" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
       <c r="M38" s="2"/>
-      <c r="N38" s="7" t="s">
+      <c r="N38" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O38" s="7"/>
-      <c r="P38" s="7"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
       <c r="Q38" s="2"/>
-      <c r="R38" s="7" t="s">
+      <c r="R38" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S38" s="7"/>
-      <c r="T38" s="7"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
       <c r="U38" s="2"/>
-      <c r="V38" s="7" t="s">
+      <c r="V38" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W38" s="7"/>
-      <c r="X38" s="7"/>
+      <c r="W38" s="10"/>
+      <c r="X38" s="10"/>
       <c r="Y38" s="2"/>
-      <c r="Z38" s="7" t="s">
+      <c r="Z38" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA38" s="7"/>
-      <c r="AB38" s="7"/>
+      <c r="AA38" s="10"/>
+      <c r="AB38" s="10"/>
       <c r="AC38" s="2"/>
-      <c r="AD38" s="7" t="s">
+      <c r="AD38" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE38" s="7"/>
-      <c r="AF38" s="7"/>
+      <c r="AE38" s="10"/>
+      <c r="AF38" s="10"/>
       <c r="AG38" s="2"/>
       <c r="AH38" s="1"/>
       <c r="AI38" s="1"/>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
-      <c r="AL38" s="7"/>
-      <c r="AM38" s="7"/>
-      <c r="AN38" s="7"/>
+      <c r="AL38" s="10"/>
+      <c r="AM38" s="10"/>
+      <c r="AN38" s="10"/>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>130</v>
+        <v>204</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -4031,7 +4028,7 @@
         <v>48</v>
       </c>
       <c r="AF39" s="1"/>
-      <c r="AG39" s="10"/>
+      <c r="AG39" s="8"/>
       <c r="AH39" s="1"/>
       <c r="AI39" s="1"/>
       <c r="AJ39" s="1"/>
@@ -4041,7 +4038,7 @@
       <c r="AN39" s="1"/>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A40" s="10"/>
+      <c r="A40" s="8"/>
       <c r="B40" s="1" t="s">
         <v>111</v>
       </c>
@@ -4105,7 +4102,7 @@
         <v>31</v>
       </c>
       <c r="AF40" s="1"/>
-      <c r="AG40" s="10"/>
+      <c r="AG40" s="8"/>
       <c r="AH40" s="1"/>
       <c r="AI40" s="1"/>
       <c r="AJ40" s="1"/>
@@ -4115,9 +4112,9 @@
       <c r="AN40" s="1"/>
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A41" s="10"/>
+      <c r="A41" s="8"/>
       <c r="B41" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>39</v>
@@ -4179,7 +4176,7 @@
         <v>20</v>
       </c>
       <c r="AF41" s="1"/>
-      <c r="AG41" s="10"/>
+      <c r="AG41" s="8"/>
       <c r="AH41" s="1"/>
       <c r="AI41" s="1"/>
       <c r="AJ41" s="1"/>
@@ -4189,9 +4186,9 @@
       <c r="AN41" s="1"/>
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A42" s="10"/>
+      <c r="A42" s="8"/>
       <c r="B42" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>8</v>
@@ -4253,7 +4250,7 @@
         <v>28</v>
       </c>
       <c r="AF42" s="1"/>
-      <c r="AG42" s="10"/>
+      <c r="AG42" s="8"/>
       <c r="AH42" s="1"/>
       <c r="AI42" s="1"/>
       <c r="AJ42" s="1"/>
@@ -4263,9 +4260,9 @@
       <c r="AN42" s="1"/>
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A43" s="10"/>
+      <c r="A43" s="8"/>
       <c r="B43" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>9</v>
@@ -4327,7 +4324,7 @@
         <v>9</v>
       </c>
       <c r="AF43" s="1"/>
-      <c r="AG43" s="10"/>
+      <c r="AG43" s="8"/>
       <c r="AH43" s="1"/>
       <c r="AI43" s="1"/>
       <c r="AJ43" s="1"/>
@@ -4337,9 +4334,9 @@
       <c r="AN43" s="1"/>
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A44" s="10"/>
+      <c r="A44" s="8"/>
       <c r="B44" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>10</v>
@@ -4401,7 +4398,7 @@
         <v>10</v>
       </c>
       <c r="AF44" s="1"/>
-      <c r="AG44" s="10"/>
+      <c r="AG44" s="8"/>
       <c r="AH44" s="1"/>
       <c r="AI44" s="1"/>
       <c r="AJ44" s="1"/>
@@ -4411,7 +4408,7 @@
       <c r="AN44" s="1"/>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A45" s="10"/>
+      <c r="A45" s="8"/>
       <c r="B45" s="1" t="s">
         <v>72</v>
       </c>
@@ -4475,7 +4472,7 @@
         <v>12</v>
       </c>
       <c r="AF45" s="1"/>
-      <c r="AG45" s="10"/>
+      <c r="AG45" s="8"/>
       <c r="AH45" s="1"/>
       <c r="AI45" s="1"/>
       <c r="AJ45" s="1"/>
@@ -4532,51 +4529,51 @@
         <v>110</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="7" t="s">
+      <c r="F47" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
       <c r="I47" s="2"/>
-      <c r="J47" s="7" t="s">
+      <c r="J47" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="10"/>
       <c r="M47" s="2"/>
-      <c r="N47" s="7" t="s">
+      <c r="N47" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O47" s="7"/>
-      <c r="P47" s="7"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
       <c r="Q47" s="2"/>
-      <c r="R47" s="7" t="s">
+      <c r="R47" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S47" s="7"/>
-      <c r="T47" s="7"/>
+      <c r="S47" s="10"/>
+      <c r="T47" s="10"/>
       <c r="U47" s="2"/>
-      <c r="V47" s="7" t="s">
+      <c r="V47" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W47" s="7"/>
-      <c r="X47" s="7"/>
+      <c r="W47" s="10"/>
+      <c r="X47" s="10"/>
       <c r="Y47" s="2"/>
-      <c r="Z47" s="7" t="s">
+      <c r="Z47" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA47" s="7"/>
-      <c r="AB47" s="7"/>
+      <c r="AA47" s="10"/>
+      <c r="AB47" s="10"/>
       <c r="AC47" s="2"/>
-      <c r="AD47" s="7" t="s">
+      <c r="AD47" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE47" s="7"/>
-      <c r="AF47" s="7"/>
+      <c r="AE47" s="10"/>
+      <c r="AF47" s="10"/>
       <c r="AG47" s="1"/>
       <c r="AH47" s="1"/>
       <c r="AI47" s="1"/>
@@ -4587,14 +4584,14 @@
       <c r="AN47" s="1"/>
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -4663,9 +4660,9 @@
       <c r="AN48" s="1"/>
     </row>
     <row r="49" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A49" s="10"/>
+      <c r="A49" s="8"/>
       <c r="B49" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>3</v>
@@ -4737,7 +4734,7 @@
       <c r="AN49" s="1"/>
     </row>
     <row r="50" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A50" s="10"/>
+      <c r="A50" s="8"/>
       <c r="B50" s="1" t="s">
         <v>112</v>
       </c>
@@ -4811,7 +4808,7 @@
       <c r="AN50" s="1"/>
     </row>
     <row r="51" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A51" s="10"/>
+      <c r="A51" s="8"/>
       <c r="B51" s="1" t="s">
         <v>117</v>
       </c>
@@ -4885,7 +4882,7 @@
       <c r="AN51" s="1"/>
     </row>
     <row r="52" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A52" s="10"/>
+      <c r="A52" s="8"/>
       <c r="B52" s="1" t="s">
         <v>118</v>
       </c>
@@ -4959,9 +4956,9 @@
       <c r="AN52" s="1"/>
     </row>
     <row r="53" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A53" s="10"/>
+      <c r="A53" s="8"/>
       <c r="B53" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>11</v>
@@ -5033,7 +5030,7 @@
       <c r="AN53" s="1"/>
     </row>
     <row r="54" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A54" s="10"/>
+      <c r="A54" s="8"/>
       <c r="B54" s="1" t="s">
         <v>72</v>
       </c>
@@ -5156,53 +5153,53 @@
         <v>110</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>110</v>
       </c>
       <c r="E56" s="1"/>
-      <c r="F56" s="7" t="s">
+      <c r="F56" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
       <c r="I56" s="2"/>
-      <c r="J56" s="7" t="s">
+      <c r="J56" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K56" s="7"/>
-      <c r="L56" s="7"/>
+      <c r="K56" s="10"/>
+      <c r="L56" s="10"/>
       <c r="M56" s="2"/>
-      <c r="N56" s="7" t="s">
+      <c r="N56" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O56" s="7"/>
-      <c r="P56" s="7"/>
+      <c r="O56" s="10"/>
+      <c r="P56" s="10"/>
       <c r="Q56" s="2"/>
-      <c r="R56" s="7" t="s">
+      <c r="R56" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S56" s="7"/>
-      <c r="T56" s="7"/>
+      <c r="S56" s="10"/>
+      <c r="T56" s="10"/>
       <c r="U56" s="2"/>
-      <c r="V56" s="7" t="s">
+      <c r="V56" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W56" s="7"/>
-      <c r="X56" s="7"/>
+      <c r="W56" s="10"/>
+      <c r="X56" s="10"/>
       <c r="Y56" s="2"/>
-      <c r="Z56" s="7" t="s">
+      <c r="Z56" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA56" s="7"/>
-      <c r="AB56" s="7"/>
+      <c r="AA56" s="10"/>
+      <c r="AB56" s="10"/>
       <c r="AC56" s="2"/>
-      <c r="AD56" s="7" t="s">
+      <c r="AD56" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE56" s="7"/>
-      <c r="AF56" s="7"/>
+      <c r="AE56" s="10"/>
+      <c r="AF56" s="10"/>
       <c r="AG56" s="1"/>
       <c r="AH56" s="1"/>
       <c r="AI56" s="1"/>
@@ -5213,17 +5210,17 @@
       <c r="AN56" s="1"/>
     </row>
     <row r="57" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A57" s="10" t="s">
+      <c r="A57" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
@@ -5305,7 +5302,7 @@
       <c r="AN57" s="1"/>
     </row>
     <row r="58" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A58" s="10"/>
+      <c r="A58" s="8"/>
       <c r="B58" s="1" t="s">
         <v>115</v>
       </c>
@@ -5395,7 +5392,7 @@
       <c r="AN58" s="1"/>
     </row>
     <row r="59" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A59" s="10"/>
+      <c r="A59" s="8"/>
       <c r="B59" s="1" t="s">
         <v>116</v>
       </c>
@@ -5403,7 +5400,7 @@
         <v>39</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
@@ -5485,7 +5482,7 @@
       <c r="AN59" s="1"/>
     </row>
     <row r="60" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A60" s="10"/>
+      <c r="A60" s="8"/>
       <c r="B60" s="1" t="s">
         <v>113</v>
       </c>
@@ -5575,7 +5572,7 @@
       <c r="AN60" s="1"/>
     </row>
     <row r="61" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A61" s="10"/>
+      <c r="A61" s="8"/>
       <c r="B61" s="1" t="s">
         <v>114</v>
       </c>
@@ -5665,9 +5662,9 @@
       <c r="AN61" s="1"/>
     </row>
     <row r="62" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A62" s="10"/>
+      <c r="A62" s="8"/>
       <c r="B62" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>10</v>
@@ -5755,7 +5752,7 @@
       <c r="AN62" s="1"/>
     </row>
     <row r="63" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A63" s="10"/>
+      <c r="A63" s="8"/>
       <c r="B63" s="1" t="s">
         <v>102</v>
       </c>
@@ -5895,50 +5892,50 @@
         <v>110</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E65" s="1"/>
-      <c r="F65" s="7" t="s">
+      <c r="F65" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G65" s="7"/>
-      <c r="H65" s="7"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
       <c r="I65" s="2"/>
-      <c r="J65" s="7" t="s">
+      <c r="J65" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K65" s="7"/>
-      <c r="L65" s="7"/>
+      <c r="K65" s="10"/>
+      <c r="L65" s="10"/>
       <c r="M65" s="2"/>
-      <c r="N65" s="7" t="s">
+      <c r="N65" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O65" s="7"/>
-      <c r="P65" s="7"/>
+      <c r="O65" s="10"/>
+      <c r="P65" s="10"/>
       <c r="Q65" s="2"/>
-      <c r="R65" s="7" t="s">
+      <c r="R65" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S65" s="7"/>
-      <c r="T65" s="7"/>
+      <c r="S65" s="10"/>
+      <c r="T65" s="10"/>
       <c r="U65" s="2"/>
-      <c r="V65" s="7" t="s">
+      <c r="V65" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W65" s="7"/>
-      <c r="X65" s="7"/>
+      <c r="W65" s="10"/>
+      <c r="X65" s="10"/>
       <c r="Y65" s="2"/>
-      <c r="Z65" s="7" t="s">
+      <c r="Z65" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA65" s="7"/>
-      <c r="AB65" s="7"/>
+      <c r="AA65" s="10"/>
+      <c r="AB65" s="10"/>
       <c r="AC65" s="2"/>
-      <c r="AD65" s="7" t="s">
+      <c r="AD65" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE65" s="7"/>
-      <c r="AF65" s="7"/>
+      <c r="AE65" s="10"/>
+      <c r="AF65" s="10"/>
       <c r="AG65" s="1"/>
       <c r="AH65" s="1"/>
       <c r="AI65" s="1"/>
@@ -5949,7 +5946,7 @@
       <c r="AN65" s="1"/>
     </row>
     <row r="66" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -5959,7 +5956,7 @@
         <v>120</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
@@ -6041,12 +6038,12 @@
       <c r="AN66" s="1"/>
     </row>
     <row r="67" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A67" s="10"/>
+      <c r="A67" s="8"/>
       <c r="B67" s="1" t="s">
         <v>126</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>3</v>
@@ -6131,9 +6128,9 @@
       <c r="AN67" s="1"/>
     </row>
     <row r="68" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A68" s="10"/>
+      <c r="A68" s="8"/>
       <c r="B68" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>113</v>
@@ -6221,9 +6218,9 @@
       <c r="AN68" s="1"/>
     </row>
     <row r="69" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A69" s="10"/>
+      <c r="A69" s="8"/>
       <c r="B69" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>69</v>
@@ -6311,7 +6308,7 @@
       <c r="AN69" s="1"/>
     </row>
     <row r="70" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A70" s="10"/>
+      <c r="A70" s="8"/>
       <c r="B70" s="1" t="s">
         <v>123</v>
       </c>
@@ -6401,7 +6398,7 @@
       <c r="AN70" s="1"/>
     </row>
     <row r="71" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A71" s="10"/>
+      <c r="A71" s="8"/>
       <c r="B71" s="1" t="s">
         <v>124</v>
       </c>
@@ -6491,7 +6488,7 @@
       <c r="AN71" s="1"/>
     </row>
     <row r="72" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A72" s="10"/>
+      <c r="A72" s="8"/>
       <c r="B72" s="1" t="s">
         <v>125</v>
       </c>
@@ -6624,9 +6621,9 @@
     </row>
     <row r="74" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -6667,52 +6664,52 @@
     <row r="75" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A75" s="2"/>
       <c r="B75" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="7" t="s">
+      <c r="F75" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G75" s="7"/>
-      <c r="H75" s="7"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
       <c r="I75" s="2"/>
-      <c r="J75" s="7" t="s">
+      <c r="J75" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K75" s="7"/>
-      <c r="L75" s="7"/>
+      <c r="K75" s="10"/>
+      <c r="L75" s="10"/>
       <c r="M75" s="2"/>
-      <c r="N75" s="7" t="s">
+      <c r="N75" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O75" s="7"/>
-      <c r="P75" s="7"/>
+      <c r="O75" s="10"/>
+      <c r="P75" s="10"/>
       <c r="Q75" s="2"/>
-      <c r="R75" s="7" t="s">
+      <c r="R75" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S75" s="7"/>
-      <c r="T75" s="7"/>
+      <c r="S75" s="10"/>
+      <c r="T75" s="10"/>
       <c r="U75" s="2"/>
-      <c r="V75" s="7" t="s">
+      <c r="V75" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W75" s="7"/>
-      <c r="X75" s="7"/>
+      <c r="W75" s="10"/>
+      <c r="X75" s="10"/>
       <c r="Y75" s="2"/>
-      <c r="Z75" s="7" t="s">
+      <c r="Z75" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA75" s="7"/>
-      <c r="AB75" s="7"/>
+      <c r="AA75" s="10"/>
+      <c r="AB75" s="10"/>
       <c r="AC75" s="2"/>
-      <c r="AD75" s="7" t="s">
+      <c r="AD75" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE75" s="7"/>
-      <c r="AF75" s="7"/>
+      <c r="AE75" s="10"/>
+      <c r="AF75" s="10"/>
       <c r="AG75" s="1"/>
       <c r="AH75" s="1"/>
       <c r="AI75" s="1"/>
@@ -6723,17 +6720,17 @@
       <c r="AN75" s="1"/>
     </row>
     <row r="76" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="8" t="s">
         <v>50</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
@@ -6783,7 +6780,7 @@
         <v>51</v>
       </c>
       <c r="X76" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y76" s="1"/>
       <c r="Z76" s="1" t="s">
@@ -6815,15 +6812,15 @@
       <c r="AN76" s="1"/>
     </row>
     <row r="77" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A77" s="10"/>
+      <c r="A77" s="8"/>
       <c r="B77" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
@@ -6905,15 +6902,15 @@
       <c r="AN77" s="1"/>
     </row>
     <row r="78" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A78" s="10"/>
+      <c r="A78" s="8"/>
       <c r="B78" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
@@ -6995,15 +6992,15 @@
       <c r="AN78" s="1"/>
     </row>
     <row r="79" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A79" s="10"/>
+      <c r="A79" s="8"/>
       <c r="B79" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
@@ -7085,15 +7082,15 @@
       <c r="AN79" s="1"/>
     </row>
     <row r="80" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A80" s="10"/>
+      <c r="A80" s="8"/>
       <c r="B80" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
@@ -7175,7 +7172,7 @@
       <c r="AN80" s="1"/>
     </row>
     <row r="81" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A81" s="10"/>
+      <c r="A81" s="8"/>
       <c r="B81" s="1" t="s">
         <v>11</v>
       </c>
@@ -7183,7 +7180,7 @@
         <v>128</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
@@ -7265,7 +7262,7 @@
       <c r="AN81" s="1"/>
     </row>
     <row r="82" spans="1:40" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="10"/>
+      <c r="A82" s="8"/>
       <c r="B82" s="1" t="s">
         <v>12</v>
       </c>
@@ -7273,7 +7270,7 @@
         <v>129</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
@@ -7398,9 +7395,9 @@
     </row>
     <row r="84" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
-      <c r="B84" s="11"/>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
@@ -7443,52 +7440,52 @@
         <v>107</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
-      <c r="F85" s="7" t="s">
+      <c r="F85" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G85" s="7"/>
-      <c r="H85" s="7"/>
+      <c r="G85" s="10"/>
+      <c r="H85" s="10"/>
       <c r="I85" s="2"/>
-      <c r="J85" s="7" t="s">
+      <c r="J85" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K85" s="7"/>
-      <c r="L85" s="7"/>
+      <c r="K85" s="10"/>
+      <c r="L85" s="10"/>
       <c r="M85" s="2"/>
-      <c r="N85" s="7" t="s">
+      <c r="N85" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O85" s="7"/>
-      <c r="P85" s="7"/>
+      <c r="O85" s="10"/>
+      <c r="P85" s="10"/>
       <c r="Q85" s="2"/>
-      <c r="R85" s="7" t="s">
+      <c r="R85" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S85" s="7"/>
-      <c r="T85" s="7"/>
+      <c r="S85" s="10"/>
+      <c r="T85" s="10"/>
       <c r="U85" s="2"/>
-      <c r="V85" s="7" t="s">
+      <c r="V85" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W85" s="7"/>
-      <c r="X85" s="7"/>
+      <c r="W85" s="10"/>
+      <c r="X85" s="10"/>
       <c r="Y85" s="2"/>
-      <c r="Z85" s="7" t="s">
+      <c r="Z85" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA85" s="7"/>
-      <c r="AB85" s="7"/>
+      <c r="AA85" s="10"/>
+      <c r="AB85" s="10"/>
       <c r="AC85" s="2"/>
-      <c r="AD85" s="7" t="s">
+      <c r="AD85" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AE85" s="7"/>
-      <c r="AF85" s="7"/>
+      <c r="AE85" s="10"/>
+      <c r="AF85" s="10"/>
       <c r="AG85" s="1"/>
       <c r="AH85" s="1"/>
       <c r="AI85" s="1"/>
@@ -7499,17 +7496,17 @@
       <c r="AN85" s="1"/>
     </row>
     <row r="86" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A86" s="10" t="s">
+      <c r="A86" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1" t="s">
@@ -7591,15 +7588,15 @@
       <c r="AN86" s="1"/>
     </row>
     <row r="87" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A87" s="10"/>
+      <c r="A87" s="8"/>
       <c r="B87" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>219</v>
-      </c>
       <c r="D87" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1" t="s">
@@ -7681,12 +7678,12 @@
       <c r="AN87" s="1"/>
     </row>
     <row r="88" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A88" s="10"/>
+      <c r="A88" s="8"/>
       <c r="B88" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>129</v>
@@ -7771,15 +7768,15 @@
       <c r="AN88" s="1"/>
     </row>
     <row r="89" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A89" s="10"/>
+      <c r="A89" s="8"/>
       <c r="B89" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1" t="s">
@@ -7861,7 +7858,7 @@
       <c r="AN89" s="1"/>
     </row>
     <row r="90" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A90" s="10"/>
+      <c r="A90" s="8"/>
       <c r="B90" s="1" t="s">
         <v>10</v>
       </c>
@@ -7869,7 +7866,7 @@
         <v>34</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1" t="s">
@@ -7951,7 +7948,7 @@
       <c r="AN90" s="1"/>
     </row>
     <row r="91" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A91" s="10"/>
+      <c r="A91" s="8"/>
       <c r="B91" s="1" t="s">
         <v>11</v>
       </c>
@@ -7959,7 +7956,7 @@
         <v>122</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
@@ -8041,7 +8038,7 @@
       <c r="AN91" s="1"/>
     </row>
     <row r="92" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A92" s="10"/>
+      <c r="A92" s="8"/>
       <c r="B92" s="1" t="s">
         <v>12</v>
       </c>
@@ -8177,32 +8174,32 @@
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E94" s="1"/>
-      <c r="F94" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
+      <c r="F94" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="G94" s="10"/>
+      <c r="H94" s="10"/>
       <c r="I94" s="2"/>
-      <c r="J94" s="7" t="s">
+      <c r="J94" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K94" s="7"/>
-      <c r="L94" s="7"/>
+      <c r="K94" s="10"/>
+      <c r="L94" s="10"/>
       <c r="M94" s="2"/>
-      <c r="N94" s="7" t="s">
+      <c r="N94" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="O94" s="7"/>
-      <c r="P94" s="7"/>
+      <c r="O94" s="10"/>
+      <c r="P94" s="10"/>
       <c r="Q94" s="2"/>
-      <c r="R94" s="7" t="s">
+      <c r="R94" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="S94" s="7"/>
-      <c r="T94" s="7"/>
+      <c r="S94" s="10"/>
+      <c r="T94" s="10"/>
       <c r="U94" s="1"/>
       <c r="V94" s="1"/>
       <c r="W94" s="1"/>
@@ -8225,57 +8222,57 @@
       <c r="AN94" s="1"/>
     </row>
     <row r="95" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="8" t="s">
-        <v>138</v>
+      <c r="A95" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G95" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G95" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="H95" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I95" s="1"/>
       <c r="J95" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K95" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="K95" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="L95" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M95" s="1"/>
       <c r="N95" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O95" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="O95" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="P95" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q95" s="1"/>
       <c r="R95" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="S95" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="S95" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="T95" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U95" s="1"/>
       <c r="V95" s="1"/>
@@ -8299,15 +8296,15 @@
       <c r="AN95" s="1"/>
     </row>
     <row r="96" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="8"/>
+      <c r="A96" s="9"/>
       <c r="B96" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1" t="s">
@@ -8371,15 +8368,15 @@
       <c r="AN96" s="1"/>
     </row>
     <row r="97" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="8"/>
+      <c r="A97" s="9"/>
       <c r="B97" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1" t="s">
@@ -8443,15 +8440,15 @@
       <c r="AN97" s="1"/>
     </row>
     <row r="98" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="8"/>
+      <c r="A98" s="9"/>
       <c r="B98" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1" t="s">
@@ -8515,15 +8512,15 @@
       <c r="AN98" s="1"/>
     </row>
     <row r="99" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="8"/>
+      <c r="A99" s="9"/>
       <c r="B99" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1" t="s">
@@ -8587,15 +8584,15 @@
       <c r="AN99" s="1"/>
     </row>
     <row r="100" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="8"/>
+      <c r="A100" s="9"/>
       <c r="B100" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1" t="s">
@@ -8659,15 +8656,15 @@
       <c r="AN100" s="1"/>
     </row>
     <row r="101" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="8"/>
+      <c r="A101" s="9"/>
       <c r="B101" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1" t="s">
@@ -8778,29 +8775,29 @@
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
-      <c r="F103" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="G103" s="7"/>
-      <c r="H103" s="7"/>
+      <c r="F103" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="G103" s="10"/>
+      <c r="H103" s="10"/>
       <c r="I103" s="2"/>
-      <c r="J103" s="7" t="s">
+      <c r="J103" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K103" s="7"/>
-      <c r="L103" s="7"/>
+      <c r="K103" s="10"/>
+      <c r="L103" s="10"/>
       <c r="M103" s="2"/>
-      <c r="N103" s="7" t="s">
+      <c r="N103" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="O103" s="7"/>
-      <c r="P103" s="7"/>
+      <c r="O103" s="10"/>
+      <c r="P103" s="10"/>
       <c r="Q103" s="2"/>
-      <c r="R103" s="7" t="s">
+      <c r="R103" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="S103" s="7"/>
-      <c r="T103" s="7"/>
+      <c r="S103" s="10"/>
+      <c r="T103" s="10"/>
       <c r="U103" s="1"/>
       <c r="V103" s="1"/>
       <c r="W103" s="1"/>
@@ -8823,48 +8820,48 @@
       <c r="AN103" s="1"/>
     </row>
     <row r="104" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="8" t="s">
+      <c r="A104" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="C104" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H104" s="1"/>
       <c r="I104" s="1"/>
       <c r="J104" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L104" s="1"/>
       <c r="M104" s="1"/>
       <c r="N104" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O104" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P104" s="1"/>
       <c r="Q104" s="1"/>
       <c r="R104" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S104" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T104" s="1"/>
       <c r="U104" s="1"/>
@@ -8889,15 +8886,15 @@
       <c r="AN104" s="1"/>
     </row>
     <row r="105" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="8"/>
+      <c r="A105" s="9"/>
       <c r="B105" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1" t="s">
@@ -8961,15 +8958,15 @@
       <c r="AN105" s="1"/>
     </row>
     <row r="106" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="8"/>
+      <c r="A106" s="9"/>
       <c r="B106" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1" t="s">
@@ -9033,15 +9030,15 @@
       <c r="AN106" s="1"/>
     </row>
     <row r="107" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="8"/>
+      <c r="A107" s="9"/>
       <c r="B107" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1" t="s">
@@ -9105,15 +9102,15 @@
       <c r="AN107" s="1"/>
     </row>
     <row r="108" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="8"/>
+      <c r="A108" s="9"/>
       <c r="B108" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1" t="s">
@@ -9177,15 +9174,15 @@
       <c r="AN108" s="1"/>
     </row>
     <row r="109" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="8"/>
+      <c r="A109" s="9"/>
       <c r="B109" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1" t="s">
@@ -9249,15 +9246,15 @@
       <c r="AN109" s="1"/>
     </row>
     <row r="110" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="8"/>
+      <c r="A110" s="9"/>
       <c r="B110" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1" t="s">
@@ -9321,7 +9318,7 @@
       <c r="AN110" s="1"/>
     </row>
     <row r="112" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A112" s="8" t="s">
+      <c r="A112" s="9" t="s">
         <v>74</v>
       </c>
       <c r="B112" s="1"/>
@@ -9341,12 +9338,12 @@
         <v>80</v>
       </c>
       <c r="H112" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I112" s="12"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A113" s="8"/>
+      <c r="A113" s="9"/>
       <c r="B113" s="1" t="s">
         <v>13</v>
       </c>
@@ -9369,7 +9366,7 @@
       <c r="I113" s="12"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A114" s="8"/>
+      <c r="A114" s="9"/>
       <c r="B114" s="1" t="s">
         <v>17</v>
       </c>
@@ -9392,7 +9389,7 @@
       <c r="I114" s="12"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A115" s="8"/>
+      <c r="A115" s="9"/>
       <c r="B115" s="1" t="s">
         <v>21</v>
       </c>
@@ -9415,7 +9412,7 @@
       <c r="I115" s="12"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A116" s="8"/>
+      <c r="A116" s="9"/>
       <c r="B116" s="1" t="s">
         <v>23</v>
       </c>
@@ -9438,7 +9435,7 @@
       <c r="I116" s="12"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A117" s="8"/>
+      <c r="A117" s="9"/>
       <c r="B117" s="1" t="s">
         <v>25</v>
       </c>
@@ -9461,7 +9458,7 @@
       <c r="I117" s="12"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A118" s="8"/>
+      <c r="A118" s="9"/>
       <c r="B118" s="1" t="s">
         <v>30</v>
       </c>
@@ -9484,7 +9481,7 @@
       <c r="I118" s="12"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A119" s="8"/>
+      <c r="A119" s="9"/>
       <c r="B119" s="1" t="s">
         <v>75</v>
       </c>
@@ -9508,14 +9505,82 @@
     </row>
   </sheetData>
   <mergeCells count="99">
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="A86:A92"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A66:A72"/>
-    <mergeCell ref="A57:A63"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="R94:T94"/>
+    <mergeCell ref="A95:A101"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="J103:L103"/>
+    <mergeCell ref="N103:P103"/>
+    <mergeCell ref="R103:T103"/>
+    <mergeCell ref="A112:A119"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="J94:L94"/>
+    <mergeCell ref="N94:P94"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="H112:I119"/>
+    <mergeCell ref="F1:AF1"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="AD11:AF11"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="V19:X19"/>
+    <mergeCell ref="Z19:AB19"/>
+    <mergeCell ref="AD19:AF19"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="V11:X11"/>
+    <mergeCell ref="Z11:AB11"/>
+    <mergeCell ref="Z29:AB29"/>
+    <mergeCell ref="AD29:AF29"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="N38:P38"/>
+    <mergeCell ref="R38:T38"/>
+    <mergeCell ref="V38:X38"/>
+    <mergeCell ref="Z38:AB38"/>
+    <mergeCell ref="AD38:AF38"/>
+    <mergeCell ref="V29:X29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="R29:T29"/>
+    <mergeCell ref="AL38:AN38"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="AG39:AG45"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="J47:L47"/>
+    <mergeCell ref="N47:P47"/>
+    <mergeCell ref="R47:T47"/>
+    <mergeCell ref="V47:X47"/>
+    <mergeCell ref="Z47:AB47"/>
+    <mergeCell ref="AD47:AF47"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="J65:L65"/>
+    <mergeCell ref="N65:P65"/>
+    <mergeCell ref="R65:T65"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="J56:L56"/>
+    <mergeCell ref="N56:P56"/>
+    <mergeCell ref="R56:T56"/>
+    <mergeCell ref="Z56:AB56"/>
+    <mergeCell ref="AD56:AF56"/>
+    <mergeCell ref="V65:X65"/>
+    <mergeCell ref="Z65:AB65"/>
+    <mergeCell ref="AD65:AF65"/>
+    <mergeCell ref="V56:X56"/>
     <mergeCell ref="Z75:AB75"/>
     <mergeCell ref="AD75:AF75"/>
     <mergeCell ref="A76:A82"/>
@@ -9531,82 +9596,14 @@
     <mergeCell ref="N75:P75"/>
     <mergeCell ref="R75:T75"/>
     <mergeCell ref="V75:X75"/>
-    <mergeCell ref="Z56:AB56"/>
-    <mergeCell ref="AD56:AF56"/>
-    <mergeCell ref="V65:X65"/>
-    <mergeCell ref="Z65:AB65"/>
-    <mergeCell ref="AD65:AF65"/>
-    <mergeCell ref="V56:X56"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="J65:L65"/>
-    <mergeCell ref="N65:P65"/>
-    <mergeCell ref="R65:T65"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="J56:L56"/>
-    <mergeCell ref="N56:P56"/>
-    <mergeCell ref="R56:T56"/>
-    <mergeCell ref="AL38:AN38"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="AG39:AG45"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="J47:L47"/>
-    <mergeCell ref="N47:P47"/>
-    <mergeCell ref="R47:T47"/>
-    <mergeCell ref="V47:X47"/>
-    <mergeCell ref="Z47:AB47"/>
-    <mergeCell ref="AD47:AF47"/>
-    <mergeCell ref="Z29:AB29"/>
-    <mergeCell ref="AD29:AF29"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="N38:P38"/>
-    <mergeCell ref="R38:T38"/>
-    <mergeCell ref="V38:X38"/>
-    <mergeCell ref="Z38:AB38"/>
-    <mergeCell ref="AD38:AF38"/>
-    <mergeCell ref="V29:X29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="AD11:AF11"/>
-    <mergeCell ref="A12:A18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="V19:X19"/>
-    <mergeCell ref="Z19:AB19"/>
-    <mergeCell ref="AD19:AF19"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="V11:X11"/>
-    <mergeCell ref="Z11:AB11"/>
-    <mergeCell ref="F1:AF1"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="AD2:AF2"/>
-    <mergeCell ref="A112:A119"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="J94:L94"/>
-    <mergeCell ref="N94:P94"/>
-    <mergeCell ref="A104:A110"/>
-    <mergeCell ref="H112:I119"/>
-    <mergeCell ref="R94:T94"/>
-    <mergeCell ref="A95:A101"/>
-    <mergeCell ref="F103:H103"/>
-    <mergeCell ref="J103:L103"/>
-    <mergeCell ref="N103:P103"/>
-    <mergeCell ref="R103:T103"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="A86:A92"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="A57:A63"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added all offensive logic checks
</commit_message>
<xml_diff>
--- a/Files/Progression Regression Logic.xlsx
+++ b/Files/Progression Regression Logic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40f61192ff96ff75/Documents/Git/madden22stats/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{4525A2FD-8FCF-4C1C-8965-B5B6FED6E457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EB4F810-B1B8-430A-B488-1632E20D0862}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{4525A2FD-8FCF-4C1C-8965-B5B6FED6E457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D06C9458-1D6B-40D0-93C4-8E9C8C749F6E}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{54C2E4B7-FBFF-4F69-A3A4-847FA497B9AB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="227">
   <si>
     <t>Yards</t>
   </si>
@@ -312,9 +312,6 @@
     <t>20-35</t>
   </si>
   <si>
-    <t>0.65+</t>
-  </si>
-  <si>
     <t>0.1-0.2</t>
   </si>
   <si>
@@ -706,6 +703,18 @@
   </si>
   <si>
     <t>35-45</t>
+  </si>
+  <si>
+    <t>0.60+</t>
+  </si>
+  <si>
+    <t>0.45-0.60</t>
+  </si>
+  <si>
+    <t>0.30-0.45</t>
+  </si>
+  <si>
+    <t>0.2-0.30</t>
   </si>
 </sst>
 </file>
@@ -798,22 +807,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1131,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39242688-C415-4EFE-B0A8-90C7EAED6EC3}">
   <dimension ref="A1:AN119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1143,42 +1152,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="26" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="11" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
@@ -1189,58 +1198,58 @@
       <c r="AN1" s="1"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="10" t="s">
+      <c r="R2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="10" t="s">
+      <c r="V2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
       <c r="Y2" s="2"/>
-      <c r="Z2" s="10" t="s">
+      <c r="Z2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
       <c r="AC2" s="2"/>
-      <c r="AD2" s="10" t="s">
+      <c r="AD2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
@@ -1251,7 +1260,7 @@
       <c r="AN2" s="2"/>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A3" s="8"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="1" t="s">
         <v>65</v>
       </c>
@@ -1341,7 +1350,7 @@
       <c r="AN3" s="1"/>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A4" s="8"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="1" t="s">
         <v>60</v>
       </c>
@@ -1431,7 +1440,7 @@
       <c r="AN4" s="1"/>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A5" s="8"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="1" t="s">
         <v>61</v>
       </c>
@@ -1521,7 +1530,7 @@
       <c r="AN5" s="1"/>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A6" s="8"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="1" t="s">
         <v>62</v>
       </c>
@@ -1611,7 +1620,7 @@
       <c r="AN6" s="1"/>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A7" s="8"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="1" t="s">
         <v>63</v>
       </c>
@@ -1701,7 +1710,7 @@
       <c r="AN7" s="1"/>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A8" s="8"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="1" t="s">
         <v>64</v>
       </c>
@@ -1791,7 +1800,7 @@
       <c r="AN8" s="1"/>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A9" s="8"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="1" t="s">
         <v>54</v>
       </c>
@@ -1803,7 +1812,7 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>26</v>
@@ -1925,54 +1934,54 @@
     <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="10" t="s">
+      <c r="N11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
       <c r="Q11" s="2"/>
-      <c r="R11" s="10" t="s">
+      <c r="R11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
       <c r="U11" s="2"/>
-      <c r="V11" s="10" t="s">
+      <c r="V11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W11" s="10"/>
-      <c r="X11" s="10"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
       <c r="Y11" s="2"/>
-      <c r="Z11" s="10" t="s">
+      <c r="Z11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA11" s="10"/>
-      <c r="AB11" s="10"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
       <c r="AC11" s="2"/>
-      <c r="AD11" s="10" t="s">
+      <c r="AD11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE11" s="10"/>
-      <c r="AF11" s="10"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
@@ -1983,7 +1992,7 @@
       <c r="AN11" s="2"/>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2059,9 +2068,9 @@
       <c r="AN12" s="1"/>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A13" s="8"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>84</v>
@@ -2133,9 +2142,9 @@
       <c r="AN13" s="1"/>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A14" s="8"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>85</v>
@@ -2207,9 +2216,9 @@
       <c r="AN14" s="1"/>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A15" s="8"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>86</v>
@@ -2281,9 +2290,9 @@
       <c r="AN15" s="1"/>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A16" s="8"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>87</v>
@@ -2355,7 +2364,7 @@
       <c r="AN16" s="1"/>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="1" t="s">
         <v>64</v>
       </c>
@@ -2429,7 +2438,7 @@
       <c r="AN17" s="1"/>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A18" s="8"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="1" t="s">
         <v>54</v>
       </c>
@@ -2439,7 +2448,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>26</v>
@@ -2508,47 +2517,47 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="10" t="s">
+      <c r="N19" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
       <c r="Q19" s="2"/>
-      <c r="R19" s="10" t="s">
+      <c r="R19" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
       <c r="U19" s="2"/>
-      <c r="V19" s="10" t="s">
+      <c r="V19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W19" s="10"/>
-      <c r="X19" s="10"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
       <c r="Y19" s="2"/>
-      <c r="Z19" s="10" t="s">
+      <c r="Z19" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA19" s="10"/>
-      <c r="AB19" s="10"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7"/>
       <c r="AC19" s="2"/>
-      <c r="AD19" s="10" t="s">
+      <c r="AD19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE19" s="10"/>
-      <c r="AF19" s="10"/>
+      <c r="AE19" s="7"/>
+      <c r="AF19" s="7"/>
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
@@ -2559,7 +2568,7 @@
       <c r="AN19" s="1"/>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2635,12 +2644,12 @@
       <c r="AN20" s="1"/>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A21" s="8"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>92</v>
+        <v>223</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2709,12 +2718,12 @@
       <c r="AN21" s="1"/>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A22" s="8"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="1" t="s">
         <v>82</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>86</v>
+        <v>224</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -2783,12 +2792,12 @@
       <c r="AN22" s="1"/>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A23" s="8"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>87</v>
+        <v>225</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -2857,12 +2866,12 @@
       <c r="AN23" s="1"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A24" s="8"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>88</v>
+        <v>226</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -2931,12 +2940,12 @@
       <c r="AN24" s="1"/>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A25" s="8"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -3005,17 +3014,17 @@
       <c r="AN25" s="1"/>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A26" s="8"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>26</v>
@@ -3122,11 +3131,11 @@
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
-      <c r="B28" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="B28" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -3170,53 +3179,53 @@
         <v>56</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="10" t="s">
+      <c r="J29" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="10" t="s">
+      <c r="N29" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
       <c r="Q29" s="2"/>
-      <c r="R29" s="10" t="s">
+      <c r="R29" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S29" s="10"/>
-      <c r="T29" s="10"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
       <c r="U29" s="2"/>
-      <c r="V29" s="10" t="s">
+      <c r="V29" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W29" s="10"/>
-      <c r="X29" s="10"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="7"/>
       <c r="Y29" s="2"/>
-      <c r="Z29" s="10" t="s">
+      <c r="Z29" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA29" s="10"/>
-      <c r="AB29" s="10"/>
+      <c r="AA29" s="7"/>
+      <c r="AB29" s="7"/>
       <c r="AC29" s="2"/>
-      <c r="AD29" s="10" t="s">
+      <c r="AD29" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE29" s="10"/>
-      <c r="AF29" s="10"/>
+      <c r="AE29" s="7"/>
+      <c r="AF29" s="7"/>
       <c r="AG29" s="1"/>
       <c r="AH29" s="1"/>
       <c r="AI29" s="1"/>
@@ -3227,17 +3236,17 @@
       <c r="AN29" s="1"/>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
@@ -3319,15 +3328,15 @@
       <c r="AN30" s="1"/>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A31" s="8"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
@@ -3409,15 +3418,15 @@
       <c r="AN31" s="1"/>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A32" s="8"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
@@ -3499,15 +3508,15 @@
       <c r="AN32" s="1"/>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A33" s="8"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
@@ -3589,15 +3598,15 @@
       <c r="AN33" s="1"/>
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A34" s="8"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
@@ -3679,15 +3688,15 @@
       <c r="AN34" s="1"/>
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A35" s="8"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
@@ -3769,25 +3778,25 @@
       <c r="AN35" s="1"/>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A36" s="8"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1" t="s">
@@ -3902,80 +3911,80 @@
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="10" t="s">
+      <c r="F38" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
       <c r="I38" s="2"/>
-      <c r="J38" s="10" t="s">
+      <c r="J38" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
       <c r="M38" s="2"/>
-      <c r="N38" s="10" t="s">
+      <c r="N38" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
       <c r="Q38" s="2"/>
-      <c r="R38" s="10" t="s">
+      <c r="R38" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S38" s="10"/>
-      <c r="T38" s="10"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
       <c r="U38" s="2"/>
-      <c r="V38" s="10" t="s">
+      <c r="V38" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W38" s="10"/>
-      <c r="X38" s="10"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="7"/>
       <c r="Y38" s="2"/>
-      <c r="Z38" s="10" t="s">
+      <c r="Z38" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA38" s="10"/>
-      <c r="AB38" s="10"/>
+      <c r="AA38" s="7"/>
+      <c r="AB38" s="7"/>
       <c r="AC38" s="2"/>
-      <c r="AD38" s="10" t="s">
+      <c r="AD38" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE38" s="10"/>
-      <c r="AF38" s="10"/>
+      <c r="AE38" s="7"/>
+      <c r="AF38" s="7"/>
       <c r="AG38" s="2"/>
       <c r="AH38" s="1"/>
       <c r="AI38" s="1"/>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
-      <c r="AL38" s="10"/>
-      <c r="AM38" s="10"/>
-      <c r="AN38" s="10"/>
+      <c r="AL38" s="7"/>
+      <c r="AM38" s="7"/>
+      <c r="AN38" s="7"/>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>48</v>
@@ -3983,7 +3992,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>48</v>
@@ -3991,7 +4000,7 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O39" s="1" t="s">
         <v>48</v>
@@ -3999,7 +4008,7 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S39" s="1" t="s">
         <v>48</v>
@@ -4007,7 +4016,7 @@
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
       <c r="V39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W39" s="1" t="s">
         <v>48</v>
@@ -4015,7 +4024,7 @@
       <c r="X39" s="1"/>
       <c r="Y39" s="1"/>
       <c r="Z39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA39" s="1" t="s">
         <v>48</v>
@@ -4023,13 +4032,13 @@
       <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
       <c r="AD39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AE39" s="1" t="s">
         <v>48</v>
       </c>
       <c r="AF39" s="1"/>
-      <c r="AG39" s="8"/>
+      <c r="AG39" s="11"/>
       <c r="AH39" s="1"/>
       <c r="AI39" s="1"/>
       <c r="AJ39" s="1"/>
@@ -4039,9 +4048,9 @@
       <c r="AN39" s="1"/>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A40" s="8"/>
+      <c r="A40" s="11"/>
       <c r="B40" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>49</v>
@@ -4103,7 +4112,7 @@
         <v>31</v>
       </c>
       <c r="AF40" s="1"/>
-      <c r="AG40" s="8"/>
+      <c r="AG40" s="11"/>
       <c r="AH40" s="1"/>
       <c r="AI40" s="1"/>
       <c r="AJ40" s="1"/>
@@ -4113,9 +4122,9 @@
       <c r="AN40" s="1"/>
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A41" s="8"/>
+      <c r="A41" s="11"/>
       <c r="B41" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>39</v>
@@ -4177,7 +4186,7 @@
         <v>20</v>
       </c>
       <c r="AF41" s="1"/>
-      <c r="AG41" s="8"/>
+      <c r="AG41" s="11"/>
       <c r="AH41" s="1"/>
       <c r="AI41" s="1"/>
       <c r="AJ41" s="1"/>
@@ -4187,9 +4196,9 @@
       <c r="AN41" s="1"/>
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A42" s="8"/>
+      <c r="A42" s="11"/>
       <c r="B42" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>8</v>
@@ -4251,7 +4260,7 @@
         <v>28</v>
       </c>
       <c r="AF42" s="1"/>
-      <c r="AG42" s="8"/>
+      <c r="AG42" s="11"/>
       <c r="AH42" s="1"/>
       <c r="AI42" s="1"/>
       <c r="AJ42" s="1"/>
@@ -4261,9 +4270,9 @@
       <c r="AN42" s="1"/>
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A43" s="8"/>
+      <c r="A43" s="11"/>
       <c r="B43" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>9</v>
@@ -4325,7 +4334,7 @@
         <v>9</v>
       </c>
       <c r="AF43" s="1"/>
-      <c r="AG43" s="8"/>
+      <c r="AG43" s="11"/>
       <c r="AH43" s="1"/>
       <c r="AI43" s="1"/>
       <c r="AJ43" s="1"/>
@@ -4335,9 +4344,9 @@
       <c r="AN43" s="1"/>
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A44" s="8"/>
+      <c r="A44" s="11"/>
       <c r="B44" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>10</v>
@@ -4399,7 +4408,7 @@
         <v>11</v>
       </c>
       <c r="AF44" s="1"/>
-      <c r="AG44" s="8"/>
+      <c r="AG44" s="11"/>
       <c r="AH44" s="1"/>
       <c r="AI44" s="1"/>
       <c r="AJ44" s="1"/>
@@ -4409,7 +4418,7 @@
       <c r="AN44" s="1"/>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A45" s="8"/>
+      <c r="A45" s="11"/>
       <c r="B45" s="1" t="s">
         <v>72</v>
       </c>
@@ -4473,7 +4482,7 @@
         <v>12</v>
       </c>
       <c r="AF45" s="1"/>
-      <c r="AG45" s="8"/>
+      <c r="AG45" s="11"/>
       <c r="AH45" s="1"/>
       <c r="AI45" s="1"/>
       <c r="AJ45" s="1"/>
@@ -4527,54 +4536,54 @@
     <row r="47" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="B47" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="10" t="s">
+      <c r="F47" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
       <c r="I47" s="2"/>
-      <c r="J47" s="10" t="s">
+      <c r="J47" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K47" s="10"/>
-      <c r="L47" s="10"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
       <c r="M47" s="2"/>
-      <c r="N47" s="10" t="s">
+      <c r="N47" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O47" s="10"/>
-      <c r="P47" s="10"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
       <c r="Q47" s="2"/>
-      <c r="R47" s="10" t="s">
+      <c r="R47" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S47" s="10"/>
-      <c r="T47" s="10"/>
+      <c r="S47" s="7"/>
+      <c r="T47" s="7"/>
       <c r="U47" s="2"/>
-      <c r="V47" s="10" t="s">
+      <c r="V47" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W47" s="10"/>
-      <c r="X47" s="10"/>
+      <c r="W47" s="7"/>
+      <c r="X47" s="7"/>
       <c r="Y47" s="2"/>
-      <c r="Z47" s="10" t="s">
+      <c r="Z47" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA47" s="10"/>
-      <c r="AB47" s="10"/>
+      <c r="AA47" s="7"/>
+      <c r="AB47" s="7"/>
       <c r="AC47" s="2"/>
-      <c r="AD47" s="10" t="s">
+      <c r="AD47" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE47" s="10"/>
-      <c r="AF47" s="10"/>
+      <c r="AE47" s="7"/>
+      <c r="AF47" s="7"/>
       <c r="AG47" s="1"/>
       <c r="AH47" s="1"/>
       <c r="AI47" s="1"/>
@@ -4585,19 +4594,19 @@
       <c r="AN47" s="1"/>
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>48</v>
@@ -4605,7 +4614,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>48</v>
@@ -4613,7 +4622,7 @@
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O48" s="1" t="s">
         <v>48</v>
@@ -4621,7 +4630,7 @@
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S48" s="1" t="s">
         <v>48</v>
@@ -4629,7 +4638,7 @@
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
       <c r="V48" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W48" s="1" t="s">
         <v>48</v>
@@ -4637,7 +4646,7 @@
       <c r="X48" s="1"/>
       <c r="Y48" s="1"/>
       <c r="Z48" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA48" s="1" t="s">
         <v>48</v>
@@ -4645,7 +4654,7 @@
       <c r="AB48" s="1"/>
       <c r="AC48" s="1"/>
       <c r="AD48" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AE48" s="1" t="s">
         <v>48</v>
@@ -4661,9 +4670,9 @@
       <c r="AN48" s="1"/>
     </row>
     <row r="49" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A49" s="8"/>
+      <c r="A49" s="11"/>
       <c r="B49" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>3</v>
@@ -4735,9 +4744,9 @@
       <c r="AN49" s="1"/>
     </row>
     <row r="50" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A50" s="8"/>
+      <c r="A50" s="11"/>
       <c r="B50" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>8</v>
@@ -4809,9 +4818,9 @@
       <c r="AN50" s="1"/>
     </row>
     <row r="51" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A51" s="8"/>
+      <c r="A51" s="11"/>
       <c r="B51" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>9</v>
@@ -4883,9 +4892,9 @@
       <c r="AN51" s="1"/>
     </row>
     <row r="52" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A52" s="8"/>
+      <c r="A52" s="11"/>
       <c r="B52" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>10</v>
@@ -4957,9 +4966,9 @@
       <c r="AN52" s="1"/>
     </row>
     <row r="53" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A53" s="8"/>
+      <c r="A53" s="11"/>
       <c r="B53" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>11</v>
@@ -5031,7 +5040,7 @@
       <c r="AN53" s="1"/>
     </row>
     <row r="54" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A54" s="8"/>
+      <c r="A54" s="11"/>
       <c r="B54" s="1" t="s">
         <v>72</v>
       </c>
@@ -5148,59 +5157,59 @@
     </row>
     <row r="56" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E56" s="1"/>
-      <c r="F56" s="10" t="s">
+      <c r="F56" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
       <c r="I56" s="2"/>
-      <c r="J56" s="10" t="s">
+      <c r="J56" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K56" s="10"/>
-      <c r="L56" s="10"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
       <c r="M56" s="2"/>
-      <c r="N56" s="10" t="s">
+      <c r="N56" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O56" s="10"/>
-      <c r="P56" s="10"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="7"/>
       <c r="Q56" s="2"/>
-      <c r="R56" s="10" t="s">
+      <c r="R56" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S56" s="10"/>
-      <c r="T56" s="10"/>
+      <c r="S56" s="7"/>
+      <c r="T56" s="7"/>
       <c r="U56" s="2"/>
-      <c r="V56" s="10" t="s">
+      <c r="V56" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W56" s="10"/>
-      <c r="X56" s="10"/>
+      <c r="W56" s="7"/>
+      <c r="X56" s="7"/>
       <c r="Y56" s="2"/>
-      <c r="Z56" s="10" t="s">
+      <c r="Z56" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA56" s="10"/>
-      <c r="AB56" s="10"/>
+      <c r="AA56" s="7"/>
+      <c r="AB56" s="7"/>
       <c r="AC56" s="2"/>
-      <c r="AD56" s="10" t="s">
+      <c r="AD56" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE56" s="10"/>
-      <c r="AF56" s="10"/>
+      <c r="AE56" s="7"/>
+      <c r="AF56" s="7"/>
       <c r="AG56" s="1"/>
       <c r="AH56" s="1"/>
       <c r="AI56" s="1"/>
@@ -5211,21 +5220,21 @@
       <c r="AN56" s="1"/>
     </row>
     <row r="57" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>48</v>
@@ -5235,7 +5244,7 @@
       </c>
       <c r="I57" s="1"/>
       <c r="J57" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>48</v>
@@ -5245,7 +5254,7 @@
       </c>
       <c r="M57" s="1"/>
       <c r="N57" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O57" s="1" t="s">
         <v>48</v>
@@ -5255,7 +5264,7 @@
       </c>
       <c r="Q57" s="1"/>
       <c r="R57" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S57" s="1" t="s">
         <v>48</v>
@@ -5265,7 +5274,7 @@
       </c>
       <c r="U57" s="1"/>
       <c r="V57" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W57" s="1" t="s">
         <v>48</v>
@@ -5275,7 +5284,7 @@
       </c>
       <c r="Y57" s="1"/>
       <c r="Z57" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA57" s="1" t="s">
         <v>48</v>
@@ -5285,7 +5294,7 @@
       </c>
       <c r="AC57" s="1"/>
       <c r="AD57" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AE57" s="1" t="s">
         <v>48</v>
@@ -5303,9 +5312,9 @@
       <c r="AN57" s="1"/>
     </row>
     <row r="58" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A58" s="8"/>
+      <c r="A58" s="11"/>
       <c r="B58" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>49</v>
@@ -5393,15 +5402,15 @@
       <c r="AN58" s="1"/>
     </row>
     <row r="59" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A59" s="8"/>
+      <c r="A59" s="11"/>
       <c r="B59" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
@@ -5483,15 +5492,15 @@
       <c r="AN59" s="1"/>
     </row>
     <row r="60" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A60" s="8"/>
+      <c r="A60" s="11"/>
       <c r="B60" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
@@ -5573,15 +5582,15 @@
       <c r="AN60" s="1"/>
     </row>
     <row r="61" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A61" s="8"/>
+      <c r="A61" s="11"/>
       <c r="B61" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
@@ -5663,9 +5672,9 @@
       <c r="AN61" s="1"/>
     </row>
     <row r="62" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A62" s="8"/>
+      <c r="A62" s="11"/>
       <c r="B62" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>10</v>
@@ -5753,9 +5762,9 @@
       <c r="AN62" s="1"/>
     </row>
     <row r="63" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A63" s="8"/>
+      <c r="A63" s="11"/>
       <c r="B63" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>36</v>
@@ -5887,56 +5896,56 @@
     <row r="65" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
       <c r="B65" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E65" s="1"/>
-      <c r="F65" s="10" t="s">
+      <c r="F65" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G65" s="10"/>
-      <c r="H65" s="10"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
       <c r="I65" s="2"/>
-      <c r="J65" s="10" t="s">
+      <c r="J65" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K65" s="10"/>
-      <c r="L65" s="10"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
       <c r="M65" s="2"/>
-      <c r="N65" s="10" t="s">
+      <c r="N65" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O65" s="10"/>
-      <c r="P65" s="10"/>
+      <c r="O65" s="7"/>
+      <c r="P65" s="7"/>
       <c r="Q65" s="2"/>
-      <c r="R65" s="10" t="s">
+      <c r="R65" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S65" s="10"/>
-      <c r="T65" s="10"/>
+      <c r="S65" s="7"/>
+      <c r="T65" s="7"/>
       <c r="U65" s="2"/>
-      <c r="V65" s="10" t="s">
+      <c r="V65" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W65" s="10"/>
-      <c r="X65" s="10"/>
+      <c r="W65" s="7"/>
+      <c r="X65" s="7"/>
       <c r="Y65" s="2"/>
-      <c r="Z65" s="10" t="s">
+      <c r="Z65" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA65" s="10"/>
-      <c r="AB65" s="10"/>
+      <c r="AA65" s="7"/>
+      <c r="AB65" s="7"/>
       <c r="AC65" s="2"/>
-      <c r="AD65" s="10" t="s">
+      <c r="AD65" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE65" s="10"/>
-      <c r="AF65" s="10"/>
+      <c r="AE65" s="7"/>
+      <c r="AF65" s="7"/>
       <c r="AG65" s="1"/>
       <c r="AH65" s="1"/>
       <c r="AI65" s="1"/>
@@ -5947,24 +5956,24 @@
       <c r="AN65" s="1"/>
     </row>
     <row r="66" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A66" s="8" t="s">
+      <c r="A66" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
         <v>47</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>48</v>
@@ -5974,7 +5983,7 @@
         <v>47</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>48</v>
@@ -5984,7 +5993,7 @@
         <v>47</v>
       </c>
       <c r="O66" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P66" s="1" t="s">
         <v>48</v>
@@ -5994,7 +6003,7 @@
         <v>47</v>
       </c>
       <c r="S66" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T66" s="1" t="s">
         <v>48</v>
@@ -6004,7 +6013,7 @@
         <v>47</v>
       </c>
       <c r="W66" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="X66" s="1" t="s">
         <v>48</v>
@@ -6014,7 +6023,7 @@
         <v>47</v>
       </c>
       <c r="AA66" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AB66" s="1" t="s">
         <v>48</v>
@@ -6024,7 +6033,7 @@
         <v>47</v>
       </c>
       <c r="AE66" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF66" s="1" t="s">
         <v>48</v>
@@ -6039,12 +6048,12 @@
       <c r="AN66" s="1"/>
     </row>
     <row r="67" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A67" s="8"/>
+      <c r="A67" s="11"/>
       <c r="B67" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>3</v>
@@ -6129,12 +6138,12 @@
       <c r="AN67" s="1"/>
     </row>
     <row r="68" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A68" s="8"/>
+      <c r="A68" s="11"/>
       <c r="B68" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>8</v>
@@ -6219,9 +6228,9 @@
       <c r="AN68" s="1"/>
     </row>
     <row r="69" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A69" s="8"/>
+      <c r="A69" s="11"/>
       <c r="B69" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>69</v>
@@ -6309,9 +6318,9 @@
       <c r="AN69" s="1"/>
     </row>
     <row r="70" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A70" s="8"/>
+      <c r="A70" s="11"/>
       <c r="B70" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>70</v>
@@ -6399,9 +6408,9 @@
       <c r="AN70" s="1"/>
     </row>
     <row r="71" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A71" s="8"/>
+      <c r="A71" s="11"/>
       <c r="B71" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>71</v>
@@ -6489,9 +6498,9 @@
       <c r="AN71" s="1"/>
     </row>
     <row r="72" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A72" s="8"/>
+      <c r="A72" s="11"/>
       <c r="B72" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>72</v>
@@ -6622,9 +6631,9 @@
     </row>
     <row r="74" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -6665,52 +6674,52 @@
     <row r="75" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A75" s="2"/>
       <c r="B75" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="10" t="s">
+      <c r="F75" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G75" s="10"/>
-      <c r="H75" s="10"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
       <c r="I75" s="2"/>
-      <c r="J75" s="10" t="s">
+      <c r="J75" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K75" s="10"/>
-      <c r="L75" s="10"/>
+      <c r="K75" s="7"/>
+      <c r="L75" s="7"/>
       <c r="M75" s="2"/>
-      <c r="N75" s="10" t="s">
+      <c r="N75" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O75" s="10"/>
-      <c r="P75" s="10"/>
+      <c r="O75" s="7"/>
+      <c r="P75" s="7"/>
       <c r="Q75" s="2"/>
-      <c r="R75" s="10" t="s">
+      <c r="R75" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S75" s="10"/>
-      <c r="T75" s="10"/>
+      <c r="S75" s="7"/>
+      <c r="T75" s="7"/>
       <c r="U75" s="2"/>
-      <c r="V75" s="10" t="s">
+      <c r="V75" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W75" s="10"/>
-      <c r="X75" s="10"/>
+      <c r="W75" s="7"/>
+      <c r="X75" s="7"/>
       <c r="Y75" s="2"/>
-      <c r="Z75" s="10" t="s">
+      <c r="Z75" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA75" s="10"/>
-      <c r="AB75" s="10"/>
+      <c r="AA75" s="7"/>
+      <c r="AB75" s="7"/>
       <c r="AC75" s="2"/>
-      <c r="AD75" s="10" t="s">
+      <c r="AD75" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE75" s="10"/>
-      <c r="AF75" s="10"/>
+      <c r="AE75" s="7"/>
+      <c r="AF75" s="7"/>
       <c r="AG75" s="1"/>
       <c r="AH75" s="1"/>
       <c r="AI75" s="1"/>
@@ -6721,17 +6730,17 @@
       <c r="AN75" s="1"/>
     </row>
     <row r="76" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A76" s="8" t="s">
+      <c r="A76" s="11" t="s">
         <v>50</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
@@ -6781,7 +6790,7 @@
         <v>51</v>
       </c>
       <c r="X76" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Y76" s="1"/>
       <c r="Z76" s="1" t="s">
@@ -6813,15 +6822,15 @@
       <c r="AN76" s="1"/>
     </row>
     <row r="77" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A77" s="8"/>
+      <c r="A77" s="11"/>
       <c r="B77" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
@@ -6903,15 +6912,15 @@
       <c r="AN77" s="1"/>
     </row>
     <row r="78" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A78" s="8"/>
+      <c r="A78" s="11"/>
       <c r="B78" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
@@ -6993,15 +7002,15 @@
       <c r="AN78" s="1"/>
     </row>
     <row r="79" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A79" s="8"/>
+      <c r="A79" s="11"/>
       <c r="B79" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
@@ -7083,15 +7092,15 @@
       <c r="AN79" s="1"/>
     </row>
     <row r="80" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A80" s="8"/>
+      <c r="A80" s="11"/>
       <c r="B80" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
@@ -7173,15 +7182,15 @@
       <c r="AN80" s="1"/>
     </row>
     <row r="81" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A81" s="8"/>
+      <c r="A81" s="11"/>
       <c r="B81" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
@@ -7263,15 +7272,15 @@
       <c r="AN81" s="1"/>
     </row>
     <row r="82" spans="1:40" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="8"/>
+      <c r="A82" s="11"/>
       <c r="B82" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
@@ -7396,9 +7405,9 @@
     </row>
     <row r="84" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
-      <c r="B84" s="7"/>
-      <c r="C84" s="7"/>
-      <c r="D84" s="7"/>
+      <c r="B84" s="12"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
@@ -7438,55 +7447,55 @@
     </row>
     <row r="85" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
-      <c r="F85" s="10" t="s">
+      <c r="F85" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G85" s="10"/>
-      <c r="H85" s="10"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
       <c r="I85" s="2"/>
-      <c r="J85" s="10" t="s">
+      <c r="J85" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K85" s="10"/>
-      <c r="L85" s="10"/>
+      <c r="K85" s="7"/>
+      <c r="L85" s="7"/>
       <c r="M85" s="2"/>
-      <c r="N85" s="10" t="s">
+      <c r="N85" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O85" s="10"/>
-      <c r="P85" s="10"/>
+      <c r="O85" s="7"/>
+      <c r="P85" s="7"/>
       <c r="Q85" s="2"/>
-      <c r="R85" s="10" t="s">
+      <c r="R85" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S85" s="10"/>
-      <c r="T85" s="10"/>
+      <c r="S85" s="7"/>
+      <c r="T85" s="7"/>
       <c r="U85" s="2"/>
-      <c r="V85" s="10" t="s">
+      <c r="V85" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W85" s="10"/>
-      <c r="X85" s="10"/>
+      <c r="W85" s="7"/>
+      <c r="X85" s="7"/>
       <c r="Y85" s="2"/>
-      <c r="Z85" s="10" t="s">
+      <c r="Z85" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AA85" s="10"/>
-      <c r="AB85" s="10"/>
+      <c r="AA85" s="7"/>
+      <c r="AB85" s="7"/>
       <c r="AC85" s="2"/>
-      <c r="AD85" s="10" t="s">
+      <c r="AD85" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE85" s="10"/>
-      <c r="AF85" s="10"/>
+      <c r="AE85" s="7"/>
+      <c r="AF85" s="7"/>
       <c r="AG85" s="1"/>
       <c r="AH85" s="1"/>
       <c r="AI85" s="1"/>
@@ -7497,17 +7506,17 @@
       <c r="AN85" s="1"/>
     </row>
     <row r="86" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A86" s="8" t="s">
+      <c r="A86" s="11" t="s">
         <v>55</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1" t="s">
@@ -7589,15 +7598,15 @@
       <c r="AN86" s="1"/>
     </row>
     <row r="87" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A87" s="8"/>
+      <c r="A87" s="11"/>
       <c r="B87" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="D87" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1" t="s">
@@ -7679,15 +7688,15 @@
       <c r="AN87" s="1"/>
     </row>
     <row r="88" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A88" s="8"/>
+      <c r="A88" s="11"/>
       <c r="B88" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1" t="s">
@@ -7769,15 +7778,15 @@
       <c r="AN88" s="1"/>
     </row>
     <row r="89" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A89" s="8"/>
+      <c r="A89" s="11"/>
       <c r="B89" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1" t="s">
@@ -7859,7 +7868,7 @@
       <c r="AN89" s="1"/>
     </row>
     <row r="90" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A90" s="8"/>
+      <c r="A90" s="11"/>
       <c r="B90" s="1" t="s">
         <v>10</v>
       </c>
@@ -7867,7 +7876,7 @@
         <v>34</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1" t="s">
@@ -7949,15 +7958,15 @@
       <c r="AN90" s="1"/>
     </row>
     <row r="91" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A91" s="8"/>
+      <c r="A91" s="11"/>
       <c r="B91" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
@@ -8039,7 +8048,7 @@
       <c r="AN91" s="1"/>
     </row>
     <row r="92" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A92" s="8"/>
+      <c r="A92" s="11"/>
       <c r="B92" s="1" t="s">
         <v>12</v>
       </c>
@@ -8047,7 +8056,7 @@
         <v>42</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
@@ -8175,32 +8184,32 @@
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E94" s="1"/>
-      <c r="F94" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="G94" s="10"/>
-      <c r="H94" s="10"/>
+      <c r="F94" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
       <c r="I94" s="2"/>
-      <c r="J94" s="10" t="s">
+      <c r="J94" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K94" s="10"/>
-      <c r="L94" s="10"/>
+      <c r="K94" s="7"/>
+      <c r="L94" s="7"/>
       <c r="M94" s="2"/>
-      <c r="N94" s="10" t="s">
+      <c r="N94" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="O94" s="10"/>
-      <c r="P94" s="10"/>
+      <c r="O94" s="7"/>
+      <c r="P94" s="7"/>
       <c r="Q94" s="2"/>
-      <c r="R94" s="10" t="s">
+      <c r="R94" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="S94" s="10"/>
-      <c r="T94" s="10"/>
+      <c r="S94" s="7"/>
+      <c r="T94" s="7"/>
       <c r="U94" s="1"/>
       <c r="V94" s="1"/>
       <c r="W94" s="1"/>
@@ -8223,57 +8232,57 @@
       <c r="AN94" s="1"/>
     </row>
     <row r="95" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="9" t="s">
-        <v>130</v>
+      <c r="A95" s="8" t="s">
+        <v>129</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G95" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G95" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="H95" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I95" s="1"/>
       <c r="J95" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K95" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="K95" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="L95" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M95" s="1"/>
       <c r="N95" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="O95" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="O95" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="P95" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q95" s="1"/>
       <c r="R95" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="S95" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="S95" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="T95" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="U95" s="1"/>
       <c r="V95" s="1"/>
@@ -8297,15 +8306,15 @@
       <c r="AN95" s="1"/>
     </row>
     <row r="96" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="9"/>
+      <c r="A96" s="8"/>
       <c r="B96" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1" t="s">
@@ -8369,15 +8378,15 @@
       <c r="AN96" s="1"/>
     </row>
     <row r="97" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="9"/>
+      <c r="A97" s="8"/>
       <c r="B97" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1" t="s">
@@ -8441,15 +8450,15 @@
       <c r="AN97" s="1"/>
     </row>
     <row r="98" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="9"/>
+      <c r="A98" s="8"/>
       <c r="B98" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1" t="s">
@@ -8513,15 +8522,15 @@
       <c r="AN98" s="1"/>
     </row>
     <row r="99" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="9"/>
+      <c r="A99" s="8"/>
       <c r="B99" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1" t="s">
@@ -8585,15 +8594,15 @@
       <c r="AN99" s="1"/>
     </row>
     <row r="100" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="9"/>
+      <c r="A100" s="8"/>
       <c r="B100" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1" t="s">
@@ -8657,15 +8666,15 @@
       <c r="AN100" s="1"/>
     </row>
     <row r="101" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="9"/>
+      <c r="A101" s="8"/>
       <c r="B101" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1" t="s">
@@ -8776,29 +8785,29 @@
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
-      <c r="F103" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="G103" s="10"/>
-      <c r="H103" s="10"/>
+      <c r="F103" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G103" s="7"/>
+      <c r="H103" s="7"/>
       <c r="I103" s="2"/>
-      <c r="J103" s="10" t="s">
+      <c r="J103" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K103" s="10"/>
-      <c r="L103" s="10"/>
+      <c r="K103" s="7"/>
+      <c r="L103" s="7"/>
       <c r="M103" s="2"/>
-      <c r="N103" s="10" t="s">
+      <c r="N103" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="O103" s="10"/>
-      <c r="P103" s="10"/>
+      <c r="O103" s="7"/>
+      <c r="P103" s="7"/>
       <c r="Q103" s="2"/>
-      <c r="R103" s="10" t="s">
+      <c r="R103" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="S103" s="10"/>
-      <c r="T103" s="10"/>
+      <c r="S103" s="7"/>
+      <c r="T103" s="7"/>
       <c r="U103" s="1"/>
       <c r="V103" s="1"/>
       <c r="W103" s="1"/>
@@ -8821,48 +8830,48 @@
       <c r="AN103" s="1"/>
     </row>
     <row r="104" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="9" t="s">
+      <c r="A104" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="C104" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H104" s="1"/>
       <c r="I104" s="1"/>
       <c r="J104" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L104" s="1"/>
       <c r="M104" s="1"/>
       <c r="N104" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O104" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P104" s="1"/>
       <c r="Q104" s="1"/>
       <c r="R104" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="S104" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="T104" s="1"/>
       <c r="U104" s="1"/>
@@ -8887,15 +8896,15 @@
       <c r="AN104" s="1"/>
     </row>
     <row r="105" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="9"/>
+      <c r="A105" s="8"/>
       <c r="B105" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1" t="s">
@@ -8959,15 +8968,15 @@
       <c r="AN105" s="1"/>
     </row>
     <row r="106" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="9"/>
+      <c r="A106" s="8"/>
       <c r="B106" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1" t="s">
@@ -9031,15 +9040,15 @@
       <c r="AN106" s="1"/>
     </row>
     <row r="107" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="9"/>
+      <c r="A107" s="8"/>
       <c r="B107" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1" t="s">
@@ -9103,15 +9112,15 @@
       <c r="AN107" s="1"/>
     </row>
     <row r="108" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="9"/>
+      <c r="A108" s="8"/>
       <c r="B108" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1" t="s">
@@ -9175,15 +9184,15 @@
       <c r="AN108" s="1"/>
     </row>
     <row r="109" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="9"/>
+      <c r="A109" s="8"/>
       <c r="B109" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1" t="s">
@@ -9247,15 +9256,15 @@
       <c r="AN109" s="1"/>
     </row>
     <row r="110" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="9"/>
+      <c r="A110" s="8"/>
       <c r="B110" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1" t="s">
@@ -9319,7 +9328,7 @@
       <c r="AN110" s="1"/>
     </row>
     <row r="112" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A112" s="9" t="s">
+      <c r="A112" s="8" t="s">
         <v>74</v>
       </c>
       <c r="B112" s="1"/>
@@ -9338,13 +9347,13 @@
       <c r="G112" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H112" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="I112" s="12"/>
+      <c r="H112" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="I112" s="9"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A113" s="9"/>
+      <c r="A113" s="8"/>
       <c r="B113" s="1" t="s">
         <v>13</v>
       </c>
@@ -9363,11 +9372,11 @@
       <c r="G113" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H113" s="12"/>
-      <c r="I113" s="12"/>
+      <c r="H113" s="9"/>
+      <c r="I113" s="9"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A114" s="9"/>
+      <c r="A114" s="8"/>
       <c r="B114" s="1" t="s">
         <v>17</v>
       </c>
@@ -9386,11 +9395,11 @@
       <c r="G114" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H114" s="12"/>
-      <c r="I114" s="12"/>
+      <c r="H114" s="9"/>
+      <c r="I114" s="9"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A115" s="9"/>
+      <c r="A115" s="8"/>
       <c r="B115" s="1" t="s">
         <v>21</v>
       </c>
@@ -9409,11 +9418,11 @@
       <c r="G115" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H115" s="12"/>
-      <c r="I115" s="12"/>
+      <c r="H115" s="9"/>
+      <c r="I115" s="9"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A116" s="9"/>
+      <c r="A116" s="8"/>
       <c r="B116" s="1" t="s">
         <v>23</v>
       </c>
@@ -9432,11 +9441,11 @@
       <c r="G116" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H116" s="12"/>
-      <c r="I116" s="12"/>
+      <c r="H116" s="9"/>
+      <c r="I116" s="9"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A117" s="9"/>
+      <c r="A117" s="8"/>
       <c r="B117" s="1" t="s">
         <v>25</v>
       </c>
@@ -9455,11 +9464,11 @@
       <c r="G117" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H117" s="12"/>
-      <c r="I117" s="12"/>
+      <c r="H117" s="9"/>
+      <c r="I117" s="9"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A118" s="9"/>
+      <c r="A118" s="8"/>
       <c r="B118" s="1" t="s">
         <v>30</v>
       </c>
@@ -9478,11 +9487,11 @@
       <c r="G118" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H118" s="12"/>
-      <c r="I118" s="12"/>
+      <c r="H118" s="9"/>
+      <c r="I118" s="9"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A119" s="9"/>
+      <c r="A119" s="8"/>
       <c r="B119" s="1" t="s">
         <v>75</v>
       </c>
@@ -9501,32 +9510,74 @@
       <c r="G119" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H119" s="12"/>
-      <c r="I119" s="12"/>
+      <c r="H119" s="9"/>
+      <c r="I119" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="99">
-    <mergeCell ref="R94:T94"/>
-    <mergeCell ref="A95:A101"/>
-    <mergeCell ref="F103:H103"/>
-    <mergeCell ref="J103:L103"/>
-    <mergeCell ref="N103:P103"/>
-    <mergeCell ref="R103:T103"/>
-    <mergeCell ref="A112:A119"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="J94:L94"/>
-    <mergeCell ref="N94:P94"/>
-    <mergeCell ref="A104:A110"/>
-    <mergeCell ref="H112:I119"/>
-    <mergeCell ref="F1:AF1"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="A86:A92"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="A57:A63"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="Z75:AB75"/>
+    <mergeCell ref="AD75:AF75"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="N85:P85"/>
+    <mergeCell ref="R85:T85"/>
+    <mergeCell ref="V85:X85"/>
+    <mergeCell ref="Z85:AB85"/>
+    <mergeCell ref="AD85:AF85"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="J75:L75"/>
+    <mergeCell ref="N75:P75"/>
+    <mergeCell ref="R75:T75"/>
+    <mergeCell ref="V75:X75"/>
+    <mergeCell ref="Z56:AB56"/>
+    <mergeCell ref="AD56:AF56"/>
+    <mergeCell ref="V65:X65"/>
+    <mergeCell ref="Z65:AB65"/>
+    <mergeCell ref="AD65:AF65"/>
+    <mergeCell ref="V56:X56"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="J65:L65"/>
+    <mergeCell ref="N65:P65"/>
+    <mergeCell ref="R65:T65"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="J56:L56"/>
+    <mergeCell ref="N56:P56"/>
+    <mergeCell ref="R56:T56"/>
+    <mergeCell ref="AL38:AN38"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="AG39:AG45"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="J47:L47"/>
+    <mergeCell ref="N47:P47"/>
+    <mergeCell ref="R47:T47"/>
+    <mergeCell ref="V47:X47"/>
+    <mergeCell ref="Z47:AB47"/>
+    <mergeCell ref="AD47:AF47"/>
+    <mergeCell ref="Z29:AB29"/>
+    <mergeCell ref="AD29:AF29"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="N38:P38"/>
+    <mergeCell ref="R38:T38"/>
+    <mergeCell ref="V38:X38"/>
+    <mergeCell ref="Z38:AB38"/>
+    <mergeCell ref="AD38:AF38"/>
+    <mergeCell ref="V29:X29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="R29:T29"/>
     <mergeCell ref="AD11:AF11"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="F19:H19"/>
@@ -9542,69 +9593,27 @@
     <mergeCell ref="R11:T11"/>
     <mergeCell ref="V11:X11"/>
     <mergeCell ref="Z11:AB11"/>
-    <mergeCell ref="Z29:AB29"/>
-    <mergeCell ref="AD29:AF29"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="N38:P38"/>
-    <mergeCell ref="R38:T38"/>
-    <mergeCell ref="V38:X38"/>
-    <mergeCell ref="Z38:AB38"/>
-    <mergeCell ref="AD38:AF38"/>
-    <mergeCell ref="V29:X29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="AL38:AN38"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="AG39:AG45"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="J47:L47"/>
-    <mergeCell ref="N47:P47"/>
-    <mergeCell ref="R47:T47"/>
-    <mergeCell ref="V47:X47"/>
-    <mergeCell ref="Z47:AB47"/>
-    <mergeCell ref="AD47:AF47"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="J65:L65"/>
-    <mergeCell ref="N65:P65"/>
-    <mergeCell ref="R65:T65"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="J56:L56"/>
-    <mergeCell ref="N56:P56"/>
-    <mergeCell ref="R56:T56"/>
-    <mergeCell ref="Z56:AB56"/>
-    <mergeCell ref="AD56:AF56"/>
-    <mergeCell ref="V65:X65"/>
-    <mergeCell ref="Z65:AB65"/>
-    <mergeCell ref="AD65:AF65"/>
-    <mergeCell ref="V56:X56"/>
-    <mergeCell ref="Z75:AB75"/>
-    <mergeCell ref="AD75:AF75"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="N85:P85"/>
-    <mergeCell ref="R85:T85"/>
-    <mergeCell ref="V85:X85"/>
-    <mergeCell ref="Z85:AB85"/>
-    <mergeCell ref="AD85:AF85"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="J75:L75"/>
-    <mergeCell ref="N75:P75"/>
-    <mergeCell ref="R75:T75"/>
-    <mergeCell ref="V75:X75"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="A86:A92"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A66:A72"/>
-    <mergeCell ref="A57:A63"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F1:AF1"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="A112:A119"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="J94:L94"/>
+    <mergeCell ref="N94:P94"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="H112:I119"/>
+    <mergeCell ref="R94:T94"/>
+    <mergeCell ref="A95:A101"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="J103:L103"/>
+    <mergeCell ref="N103:P103"/>
+    <mergeCell ref="R103:T103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>